<commit_message>
Updated data from rest of Countries
</commit_message>
<xml_diff>
--- a/Sources/Paises.xlsx
+++ b/Sources/Paises.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nuria\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\PowerBI_Covid\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160F02EA-E53A-471E-8C8D-73B342AE9616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="1"/>
+    <workbookView xWindow="4050" yWindow="285" windowWidth="20490" windowHeight="15915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,10 +19,18 @@
     <sheet name="MP200pmillon" sheetId="3" r:id="rId4"/>
     <sheet name="MP500pmillon" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -177,7 +186,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -215,7 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -224,10 +233,11 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -243,9 +253,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -257,7 +267,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -283,7 +292,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -335,6 +344,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-2A41-4DC2-8406-11A6ED7132E7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:xVal>
             <c:numRef>
@@ -681,10 +695,21 @@
                 <c:pt idx="51">
                   <c:v>117710</c:v>
                 </c:pt>
+                <c:pt idx="52">
+                  <c:v>124736</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>130759</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2A41-4DC2-8406-11A6ED7132E7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1084,10 +1109,24 @@
                 <c:pt idx="49">
                   <c:v>13614</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>13614</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>15723</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>16627</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2A41-4DC2-8406-11A6ED7132E7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1131,6 +1170,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-2A41-4DC2-8406-11A6ED7132E7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:xVal>
             <c:numRef>
@@ -1305,10 +1349,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$55</c:f>
+              <c:f>Sheet1!$D$2:$D$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1461,11 +1505,22 @@
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>115242</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>119827</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>124632</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-2A41-4DC2-8406-11A6ED7132E7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1847,10 +1902,24 @@
                 <c:pt idx="49">
                   <c:v>73522</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>73522</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>79696</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>85778</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-2A41-4DC2-8406-11A6ED7132E7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1894,6 +1963,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-2A41-4DC2-8406-11A6ED7132E7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:xVal>
             <c:numRef>
@@ -2252,10 +2326,21 @@
                 <c:pt idx="50">
                   <c:v>59105</c:v>
                 </c:pt>
+                <c:pt idx="51">
+                  <c:v>64338</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>68605</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-2A41-4DC2-8406-11A6ED7132E7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -2658,10 +2743,21 @@
                 <c:pt idx="50">
                   <c:v>33718</c:v>
                 </c:pt>
+                <c:pt idx="51">
+                  <c:v>38168</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>41903</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-2A41-4DC2-8406-11A6ED7132E7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -2762,7 +2858,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$40:$H$47</c:f>
+              <c:f>Sheet1!$H$41:$H$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2794,6 +2890,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-2A41-4DC2-8406-11A6ED7132E7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2861,7 +2962,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-466491120"/>
@@ -2924,7 +3025,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-466484048"/>
@@ -2941,7 +3042,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2967,7 +3067,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2997,7 +3097,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3009,9 +3109,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3023,7 +3123,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3049,7 +3148,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3253,6 +3352,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C2B8-49E8-B282-B9D73C506EF9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3320,7 +3424,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-466487312"/>
@@ -3382,7 +3486,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-466488400"/>
@@ -3423,7 +3527,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3435,9 +3539,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3449,7 +3553,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3475,7 +3578,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3545,6 +3648,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C9BA-49C4-A6F4-2221ADF479D7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3605,6 +3713,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C9BA-49C4-A6F4-2221ADF479D7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3660,7 +3773,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-466486768"/>
@@ -3719,7 +3832,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-466482416"/>
@@ -3736,7 +3849,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3762,7 +3874,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3792,7 +3904,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3804,9 +3916,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3818,7 +3930,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3844,7 +3955,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4227,7 +4338,7 @@
                   <c:v>2522.717531075868</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0</c:v>
+                  <c:v>2802.3789112730392</c:v>
                 </c:pt>
                 <c:pt idx="54">
                   <c:v>0</c:v>
@@ -4257,6 +4368,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CE0E-46FB-BB58-D9138C5D1056}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4639,12 +4755,17 @@
                   <c:v>792.43306169965081</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>792.43306169965081</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CE0E-46FB-BB58-D9138C5D1056}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -5003,6 +5124,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CE0E-46FB-BB58-D9138C5D1056}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -5385,12 +5511,17 @@
                   <c:v>888.05411281555735</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>888.05411281555735</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-CE0E-46FB-BB58-D9138C5D1056}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -5776,6 +5907,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-CE0E-46FB-BB58-D9138C5D1056}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -6182,6 +6318,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-CE0E-46FB-BB58-D9138C5D1056}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -6329,15 +6470,20 @@
                   <c:v>568.76833740831296</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>651.41809290953552</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-CE0E-46FB-BB58-D9138C5D1056}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -6406,7 +6552,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-506307184"/>
@@ -6469,7 +6615,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-466483504"/>
@@ -6486,7 +6632,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6512,7 +6657,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6542,7 +6687,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6554,9 +6699,9 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6568,7 +6713,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6594,7 +6738,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6980,6 +7124,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F8A1-4C6C-97A5-810688E00B2C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -7365,12 +7514,17 @@
                   <c:v>792.43306169965081</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>792.43306169965081</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F8A1-4C6C-97A5-810688E00B2C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -7732,6 +7886,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F8A1-4C6C-97A5-810688E00B2C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -8114,12 +8273,17 @@
                   <c:v>888.05411281555735</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>888.05411281555735</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F8A1-4C6C-97A5-810688E00B2C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -8508,6 +8672,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F8A1-4C6C-97A5-810688E00B2C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -8914,6 +9083,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-F8A1-4C6C-97A5-810688E00B2C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -9052,15 +9226,20 @@
                   <c:v>568.76833740831296</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>651.41809290953552</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-F8A1-4C6C-97A5-810688E00B2C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -9129,7 +9308,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-666786224"/>
@@ -9192,7 +9371,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-506304464"/>
@@ -9209,7 +9388,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9235,7 +9413,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9265,7 +9443,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9277,9 +9455,9 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -9291,7 +9469,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9317,7 +9494,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9658,6 +9835,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E793-406E-B572-319052D6B66B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -9980,12 +10162,17 @@
                   <c:v>792.43306169965081</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>792.43306169965081</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E793-406E-B572-319052D6B66B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -10344,6 +10531,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E793-406E-B572-319052D6B66B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -10651,12 +10843,17 @@
                   <c:v>888.05411281555735</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>888.05411281555735</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E793-406E-B572-319052D6B66B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -10967,6 +11164,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E793-406E-B572-319052D6B66B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -11220,6 +11422,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E793-406E-B572-319052D6B66B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -11397,15 +11604,20 @@
                   <c:v>568.76833740831296</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>651.41809290953552</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-E793-406E-B572-319052D6B66B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -11474,7 +11686,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-466486224"/>
@@ -11537,7 +11749,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-666790576"/>
@@ -11554,7 +11766,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11580,7 +11791,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -11610,7 +11821,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -14961,7 +15172,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -14991,7 +15208,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -15026,7 +15249,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -15061,7 +15290,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -15098,7 +15333,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -15135,7 +15376,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -15417,21 +15664,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL70"/>
   <sheetViews>
-    <sheetView topLeftCell="R3" zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AF41" sqref="AF41"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41:H51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -15457,7 +15704,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43873</v>
       </c>
@@ -15496,7 +15743,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43874</v>
       </c>
@@ -15538,7 +15785,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43875</v>
       </c>
@@ -15580,7 +15827,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43876</v>
       </c>
@@ -15616,7 +15863,7 @@
       <c r="AB5" s="3"/>
       <c r="AD5" s="2"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43877</v>
       </c>
@@ -15655,7 +15902,7 @@
       </c>
       <c r="AD6" s="2"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43878</v>
       </c>
@@ -15697,7 +15944,7 @@
       </c>
       <c r="AD7" s="2"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43879</v>
       </c>
@@ -15746,7 +15993,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43880</v>
       </c>
@@ -15795,7 +16042,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43881</v>
       </c>
@@ -15844,7 +16091,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43882</v>
       </c>
@@ -15897,7 +16144,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43883</v>
       </c>
@@ -15936,7 +16183,7 @@
       </c>
       <c r="AD12" s="2"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43884</v>
       </c>
@@ -15975,7 +16222,7 @@
       </c>
       <c r="AD13" s="2"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43885</v>
       </c>
@@ -16026,7 +16273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43886</v>
       </c>
@@ -16083,7 +16330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43887</v>
       </c>
@@ -16143,7 +16390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43888</v>
       </c>
@@ -16210,7 +16457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43889</v>
       </c>
@@ -16277,7 +16524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43890</v>
       </c>
@@ -16341,7 +16588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43891</v>
       </c>
@@ -16412,7 +16659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43892</v>
       </c>
@@ -16486,7 +16733,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43893</v>
       </c>
@@ -16560,7 +16807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43894</v>
       </c>
@@ -16634,7 +16881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43895</v>
       </c>
@@ -16708,7 +16955,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43896</v>
       </c>
@@ -16783,7 +17030,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43897</v>
       </c>
@@ -16854,7 +17101,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43898</v>
       </c>
@@ -16926,7 +17173,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43899</v>
       </c>
@@ -17000,7 +17247,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43900</v>
       </c>
@@ -17074,7 +17321,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43901</v>
       </c>
@@ -17148,7 +17395,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43902</v>
       </c>
@@ -17222,7 +17469,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43903</v>
       </c>
@@ -17296,7 +17543,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43904</v>
       </c>
@@ -17371,7 +17618,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43905</v>
       </c>
@@ -17445,7 +17692,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43906</v>
       </c>
@@ -17519,7 +17766,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43907</v>
       </c>
@@ -17593,7 +17840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43908</v>
       </c>
@@ -17664,10 +17911,10 @@
         <v>43921</v>
       </c>
       <c r="AL37">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43909</v>
       </c>
@@ -17738,10 +17985,10 @@
         <v>43922</v>
       </c>
       <c r="AL38">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43910</v>
       </c>
@@ -17809,10 +18056,10 @@
         <v>43923</v>
       </c>
       <c r="AL39">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43911</v>
       </c>
@@ -17833,9 +18080,6 @@
       </c>
       <c r="G40">
         <v>5018</v>
-      </c>
-      <c r="H40">
-        <v>15219</v>
       </c>
       <c r="Y40">
         <v>105792</v>
@@ -17864,8 +18108,14 @@
         <f t="shared" si="26"/>
         <v>-94417</v>
       </c>
-    </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AK40" s="1">
+        <v>43924</v>
+      </c>
+      <c r="AL40">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43912</v>
       </c>
@@ -17887,8 +18137,8 @@
       <c r="G41">
         <v>5683</v>
       </c>
-      <c r="H41">
-        <v>33404</v>
+      <c r="H41" s="8">
+        <v>15219</v>
       </c>
       <c r="Y41">
         <v>110574</v>
@@ -17917,8 +18167,14 @@
         <f t="shared" si="26"/>
         <v>-102136</v>
       </c>
-    </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AK41" s="1">
+        <v>43925</v>
+      </c>
+      <c r="AL41">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43913</v>
       </c>
@@ -17940,11 +18196,17 @@
       <c r="G42">
         <v>6650</v>
       </c>
-      <c r="H42">
-        <v>44183</v>
-      </c>
-    </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="H42" s="8">
+        <v>33404</v>
+      </c>
+      <c r="AK42" s="1">
+        <v>43926</v>
+      </c>
+      <c r="AL42">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43914</v>
       </c>
@@ -17966,11 +18228,11 @@
       <c r="G43">
         <v>8077</v>
       </c>
-      <c r="H43">
-        <v>54453</v>
-      </c>
-    </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="H43" s="8">
+        <v>44183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43915</v>
       </c>
@@ -17992,11 +18254,11 @@
       <c r="G44">
         <v>9529</v>
       </c>
-      <c r="H44">
-        <v>68440</v>
-      </c>
-    </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="H44" s="8">
+        <v>54453</v>
+      </c>
+    </row>
+    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43916</v>
       </c>
@@ -18018,11 +18280,11 @@
       <c r="G45">
         <v>11658</v>
       </c>
-      <c r="H45">
-        <v>85356</v>
-      </c>
-    </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="H45" s="8">
+        <v>68440</v>
+      </c>
+    </row>
+    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43917</v>
       </c>
@@ -18044,11 +18306,11 @@
       <c r="G46">
         <v>14543</v>
       </c>
-      <c r="H46">
-        <v>103321</v>
-      </c>
-    </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="H46" s="8">
+        <v>85356</v>
+      </c>
+    </row>
+    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43918</v>
       </c>
@@ -18070,11 +18332,11 @@
       <c r="G47">
         <v>17089</v>
       </c>
-      <c r="H47">
-        <v>124665</v>
-      </c>
-    </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="H47" s="8">
+        <v>103321</v>
+      </c>
+    </row>
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43919</v>
       </c>
@@ -18096,11 +18358,11 @@
       <c r="G48">
         <v>19522</v>
       </c>
-      <c r="H48">
-        <v>143025</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H48" s="8">
+        <v>124665</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43920</v>
       </c>
@@ -18122,11 +18384,11 @@
       <c r="G49">
         <v>22141</v>
       </c>
-      <c r="H49">
-        <v>163539</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H49" s="8">
+        <v>143025</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43921</v>
       </c>
@@ -18148,11 +18410,11 @@
       <c r="G50">
         <v>25150</v>
       </c>
-      <c r="H50">
-        <v>186101</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H50" s="8">
+        <v>163539</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43922</v>
       </c>
@@ -18174,141 +18436,193 @@
       <c r="G51">
         <v>29474</v>
       </c>
-      <c r="H51">
-        <v>213144</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H51" s="8">
+        <v>186101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43923</v>
       </c>
       <c r="B52">
         <v>110238</v>
       </c>
+      <c r="C52">
+        <v>13614</v>
+      </c>
       <c r="D52">
         <v>115242</v>
       </c>
+      <c r="E52">
+        <v>73522</v>
+      </c>
       <c r="F52">
         <v>59105</v>
       </c>
       <c r="G52">
         <v>33718</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H52">
+        <v>213144</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43924</v>
       </c>
       <c r="B53">
         <v>117710</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <v>15723</v>
+      </c>
+      <c r="D53">
+        <v>119827</v>
+      </c>
+      <c r="E53">
+        <v>79696</v>
+      </c>
+      <c r="F53">
+        <v>64338</v>
+      </c>
+      <c r="G53">
+        <v>38168</v>
+      </c>
+      <c r="H53">
+        <v>239279</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43925</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>124736</v>
+      </c>
+      <c r="C54">
+        <v>16627</v>
+      </c>
+      <c r="D54">
+        <v>124632</v>
+      </c>
+      <c r="E54">
+        <v>85778</v>
+      </c>
+      <c r="F54">
+        <v>68605</v>
+      </c>
+      <c r="G54">
+        <v>41903</v>
+      </c>
+      <c r="H54">
+        <v>277205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43926</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>130759</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43927</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43928</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43929</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43930</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43931</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43932</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43933</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43934</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43935</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>43936</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>43937</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>43938</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>43939</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>43940</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>43941</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="68" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="68" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="8.88671875" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" customWidth="1"/>
     <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -18322,7 +18636,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -18354,7 +18668,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -18436,7 +18750,7 @@
         <v>0.7261574756708935</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -18518,7 +18832,7 @@
         <v>0.16119138897080504</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -18600,7 +18914,7 @@
         <v>0.11265113535830137</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -18660,7 +18974,7 @@
         <v>16565.000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -18704,7 +19018,7 @@
         <v>0.16119138897080504</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -18748,7 +19062,7 @@
         <v>0.11265113535830137</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -18803,7 +19117,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -18863,7 +19177,7 @@
         <v>94.91293272537817</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -18919,7 +19233,7 @@
         <v>252.47520218373623</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -18985,7 +19299,7 @@
         <v>0.82120201603482734</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>SUM(B3:B12)</f>
         <v>17116</v>
@@ -19015,7 +19329,7 @@
         <v>0.17935222317899052</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="Y14" s="2"/>
     </row>
   </sheetData>
@@ -19025,24 +19339,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ70"/>
   <sheetViews>
-    <sheetView topLeftCell="F6" zoomScale="84" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="F19" zoomScale="84" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Y37" sqref="Y37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>33</v>
       </c>
@@ -19068,7 +19382,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -19115,7 +19429,7 @@
         <v>0.12040939193257075</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -19164,7 +19478,7 @@
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -19213,7 +19527,7 @@
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -19262,7 +19576,7 @@
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -19311,7 +19625,7 @@
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -19361,7 +19675,7 @@
       <c r="AH7" s="2"/>
       <c r="AJ7" s="2"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -19411,7 +19725,7 @@
       <c r="AH8" s="2"/>
       <c r="AJ8" s="2"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -19461,7 +19775,7 @@
       <c r="AH9" s="2"/>
       <c r="AJ9" s="2"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -19511,7 +19825,7 @@
       <c r="AH10" s="2"/>
       <c r="AJ10" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -19559,7 +19873,7 @@
       </c>
       <c r="AJ11" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -19607,7 +19921,7 @@
       </c>
       <c r="AJ12" s="2"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -19655,7 +19969,7 @@
       </c>
       <c r="AJ13" s="2"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -19703,7 +20017,7 @@
       </c>
       <c r="AJ14" s="2"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -19751,7 +20065,7 @@
       </c>
       <c r="AJ15" s="2"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -19799,7 +20113,7 @@
       </c>
       <c r="AJ16" s="2"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -19847,7 +20161,7 @@
       </c>
       <c r="AJ17" s="2"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -19895,7 +20209,7 @@
       </c>
       <c r="AJ18" s="2"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -19936,7 +20250,7 @@
       </c>
       <c r="AJ19" s="2"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -19979,7 +20293,7 @@
       <c r="AH20" s="2"/>
       <c r="AJ20" s="2"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -20029,7 +20343,7 @@
       <c r="AH21" s="3"/>
       <c r="AJ21" s="2"/>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -20079,7 +20393,7 @@
       <c r="AH22" s="3"/>
       <c r="AJ22" s="2"/>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -20129,7 +20443,7 @@
       <c r="AH23" s="3"/>
       <c r="AJ23" s="2"/>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -20179,7 +20493,7 @@
       <c r="AH24" s="3"/>
       <c r="AJ24" s="2"/>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -20230,7 +20544,7 @@
       <c r="AH25" s="3"/>
       <c r="AJ25" s="2"/>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -20273,7 +20587,7 @@
       <c r="AH26" s="3"/>
       <c r="AJ26" s="2"/>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -20317,7 +20631,7 @@
       <c r="AH27" s="3"/>
       <c r="AJ27" s="2"/>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -20367,7 +20681,7 @@
       <c r="AH28" s="3"/>
       <c r="AJ28" s="2"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -20417,7 +20731,7 @@
       <c r="AH29" s="3"/>
       <c r="AJ29" s="2"/>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -20467,7 +20781,7 @@
       <c r="AH30" s="3"/>
       <c r="AJ30" s="2"/>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -20517,7 +20831,7 @@
       <c r="AH31" s="3"/>
       <c r="AJ31" s="2"/>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>31</v>
       </c>
@@ -20567,7 +20881,7 @@
       <c r="AH32" s="3"/>
       <c r="AJ32" s="2"/>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -20618,7 +20932,7 @@
       <c r="AH33" s="3"/>
       <c r="AJ33" s="2"/>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -20668,7 +20982,7 @@
       <c r="AH34" s="3"/>
       <c r="AJ34" s="2"/>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>34</v>
       </c>
@@ -20718,7 +21032,7 @@
       <c r="AH35" s="3"/>
       <c r="AJ35" s="2"/>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -20768,7 +21082,7 @@
       <c r="AH36" s="3"/>
       <c r="AJ36" s="2"/>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -20818,7 +21132,7 @@
       <c r="AH37" s="3"/>
       <c r="AJ37" s="2"/>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>37</v>
       </c>
@@ -20868,7 +21182,7 @@
       <c r="AH38" s="3"/>
       <c r="AJ38" s="2"/>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>38</v>
       </c>
@@ -20918,7 +21232,7 @@
       <c r="AH39" s="3"/>
       <c r="AJ39" s="2"/>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -20975,7 +21289,7 @@
       <c r="AH40" s="3"/>
       <c r="AJ40" s="2"/>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>40</v>
       </c>
@@ -21032,7 +21346,7 @@
       <c r="AH41" s="3"/>
       <c r="AJ41" s="2"/>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -21089,7 +21403,7 @@
       <c r="AH42" s="3"/>
       <c r="AJ42" s="2"/>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -21146,7 +21460,7 @@
       <c r="AH43" s="3"/>
       <c r="AJ43" s="2"/>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>43</v>
       </c>
@@ -21203,7 +21517,7 @@
       <c r="AH44" s="3"/>
       <c r="AJ44" s="2"/>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>44</v>
       </c>
@@ -21260,7 +21574,7 @@
       <c r="AH45" s="3"/>
       <c r="AJ45" s="2"/>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -21322,7 +21636,7 @@
       <c r="AH46" s="3"/>
       <c r="AJ46" s="2"/>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -21385,7 +21699,7 @@
       <c r="AH47" s="3"/>
       <c r="AJ47" s="2"/>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>47</v>
       </c>
@@ -21438,7 +21752,7 @@
         <v>293.82901866345577</v>
       </c>
       <c r="N48">
-        <f>Sheet1!H48</f>
+        <f>Sheet1!H49</f>
         <v>143025</v>
       </c>
       <c r="O48">
@@ -21449,7 +21763,7 @@
       <c r="AH48" s="3"/>
       <c r="AJ48" s="2"/>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -21502,7 +21816,7 @@
         <v>333.2480433473811</v>
       </c>
       <c r="N49">
-        <f>Sheet1!H49</f>
+        <f>Sheet1!H50</f>
         <v>163539</v>
       </c>
       <c r="O49">
@@ -21513,7 +21827,7 @@
       <c r="AH49" s="3"/>
       <c r="AJ49" s="2"/>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -21566,7 +21880,7 @@
         <v>378.53702588801929</v>
       </c>
       <c r="N50">
-        <f>Sheet1!H50</f>
+        <f>Sheet1!H51</f>
         <v>186101</v>
       </c>
       <c r="O50">
@@ -21577,7 +21891,7 @@
       <c r="AH50" s="3"/>
       <c r="AJ50" s="2"/>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>50</v>
       </c>
@@ -21629,19 +21943,19 @@
         <f t="shared" si="5"/>
         <v>443.61830222757379</v>
       </c>
-      <c r="N51">
-        <f>Sheet1!H51</f>
-        <v>213144</v>
-      </c>
-      <c r="O51">
+      <c r="N51" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O51" t="e">
         <f t="shared" si="6"/>
-        <v>651.41809290953552</v>
+        <v>#REF!</v>
       </c>
       <c r="AG51" s="2"/>
       <c r="AH51" s="3"/>
       <c r="AJ51" s="2"/>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>51</v>
       </c>
@@ -21655,11 +21969,11 @@
       </c>
       <c r="D52">
         <f>Sheet1!C52</f>
-        <v>0</v>
+        <v>13614</v>
       </c>
       <c r="E52">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>792.43306169965081</v>
       </c>
       <c r="F52">
         <f>Sheet1!D52</f>
@@ -21671,11 +21985,11 @@
       </c>
       <c r="H52">
         <f>Sheet1!E52</f>
-        <v>0</v>
+        <v>73522</v>
       </c>
       <c r="I52">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>888.05411281555735</v>
       </c>
       <c r="J52">
         <f>Sheet1!F52</f>
@@ -21695,16 +22009,16 @@
       </c>
       <c r="N52">
         <f>Sheet1!H52</f>
-        <v>0</v>
+        <v>213144</v>
       </c>
       <c r="O52">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>651.41809290953552</v>
       </c>
       <c r="AG52" s="2"/>
       <c r="AH52" s="3"/>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>52</v>
       </c>
@@ -21718,100 +22032,100 @@
       </c>
       <c r="D53">
         <f>Sheet1!C53</f>
-        <v>0</v>
+        <v>15723</v>
       </c>
       <c r="F53">
         <f>Sheet1!D53</f>
-        <v>0</v>
-      </c>
-      <c r="H53">
+        <v>119827</v>
+      </c>
+      <c r="H53" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J53">
         <f>Sheet1!E53</f>
-        <v>0</v>
-      </c>
-      <c r="J53">
-        <f>Sheet1!F53</f>
-        <v>0</v>
+        <v>79696</v>
       </c>
       <c r="L53">
         <f>Sheet1!G53</f>
-        <v>0</v>
+        <v>38168</v>
       </c>
       <c r="N53">
         <f>Sheet1!H53</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+        <v>239279</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>53</v>
       </c>
       <c r="B54">
         <f>Sheet1!B54</f>
-        <v>0</v>
+        <v>124736</v>
       </c>
       <c r="D54">
         <f>Sheet1!C54</f>
-        <v>0</v>
-      </c>
-      <c r="F54">
-        <f>Sheet1!D54</f>
-        <v>0</v>
-      </c>
-      <c r="H54">
-        <f>Sheet1!E54</f>
-        <v>0</v>
-      </c>
-      <c r="J54">
-        <f>Sheet1!F54</f>
-        <v>0</v>
-      </c>
-      <c r="L54">
-        <f>Sheet1!G54</f>
-        <v>0</v>
+        <v>16627</v>
+      </c>
+      <c r="F54" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H54" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J54" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L54" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="N54">
         <f>Sheet1!H54</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
+        <v>277205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>54</v>
       </c>
       <c r="B55">
         <f>Sheet1!B55</f>
-        <v>0</v>
+        <v>130759</v>
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2802.3789112730392</v>
       </c>
       <c r="D55">
         <f>Sheet1!C55</f>
         <v>0</v>
       </c>
       <c r="F55">
-        <f>Sheet1!D55</f>
-        <v>0</v>
+        <f>Sheet1!D54</f>
+        <v>124632</v>
       </c>
       <c r="H55">
-        <f>Sheet1!E55</f>
-        <v>0</v>
+        <f>Sheet1!E54</f>
+        <v>85778</v>
       </c>
       <c r="J55">
-        <f>Sheet1!F55</f>
-        <v>0</v>
+        <f>Sheet1!F54</f>
+        <v>68605</v>
       </c>
       <c r="L55">
-        <f>Sheet1!G55</f>
-        <v>0</v>
+        <f>Sheet1!G54</f>
+        <v>41903</v>
       </c>
       <c r="N55">
         <f>Sheet1!H55</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>55</v>
       </c>
@@ -21848,7 +22162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>56</v>
       </c>
@@ -21885,7 +22199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>57</v>
       </c>
@@ -21922,7 +22236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>58</v>
       </c>
@@ -21959,7 +22273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>59</v>
       </c>
@@ -21996,7 +22310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>60</v>
       </c>
@@ -22033,7 +22347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>61</v>
       </c>
@@ -22070,7 +22384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>62</v>
       </c>
@@ -22107,7 +22421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>63</v>
       </c>
@@ -22144,7 +22458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>64</v>
       </c>
@@ -22181,7 +22495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>65</v>
       </c>
@@ -22218,7 +22532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>66</v>
       </c>
@@ -22255,7 +22569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>67</v>
       </c>
@@ -22292,7 +22606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>68</v>
       </c>
@@ -22329,7 +22643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>69</v>
       </c>
@@ -22373,24 +22687,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AJ70"/>
   <sheetViews>
     <sheetView topLeftCell="E2" zoomScale="71" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C52" sqref="C52:C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>33</v>
       </c>
@@ -22416,7 +22730,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -22463,7 +22777,7 @@
         <v>0.12040939193257075</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -22512,7 +22826,7 @@
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -22561,7 +22875,7 @@
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -22610,7 +22924,7 @@
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -22659,7 +22973,7 @@
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -22709,7 +23023,7 @@
       <c r="AH7" s="2"/>
       <c r="AJ7" s="2"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -22759,7 +23073,7 @@
       <c r="AH8" s="2"/>
       <c r="AJ8" s="2"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -22809,7 +23123,7 @@
       <c r="AH9" s="2"/>
       <c r="AJ9" s="2"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -22859,7 +23173,7 @@
       <c r="AH10" s="2"/>
       <c r="AJ10" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -22907,7 +23221,7 @@
       </c>
       <c r="AJ11" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -22955,7 +23269,7 @@
       </c>
       <c r="AJ12" s="2"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -23003,7 +23317,7 @@
       </c>
       <c r="AJ13" s="2"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -23051,7 +23365,7 @@
       </c>
       <c r="AJ14" s="2"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -23099,7 +23413,7 @@
       </c>
       <c r="AJ15" s="2"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -23147,7 +23461,7 @@
       </c>
       <c r="AJ16" s="2"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -23195,7 +23509,7 @@
       </c>
       <c r="AJ17" s="2"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -23243,7 +23557,7 @@
       </c>
       <c r="AJ18" s="2"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -23284,7 +23598,7 @@
       </c>
       <c r="AJ19" s="2"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -23327,7 +23641,7 @@
       <c r="AH20" s="2"/>
       <c r="AJ20" s="2"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -23377,7 +23691,7 @@
       <c r="AH21" s="3"/>
       <c r="AJ21" s="2"/>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -23427,7 +23741,7 @@
       <c r="AH22" s="3"/>
       <c r="AJ22" s="2"/>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -23477,7 +23791,7 @@
       <c r="AH23" s="3"/>
       <c r="AJ23" s="2"/>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -23527,7 +23841,7 @@
       <c r="AH24" s="3"/>
       <c r="AJ24" s="2"/>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -23578,7 +23892,7 @@
       <c r="AH25" s="3"/>
       <c r="AJ25" s="2"/>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -23621,7 +23935,7 @@
       <c r="AH26" s="3"/>
       <c r="AJ26" s="2"/>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -23665,7 +23979,7 @@
       <c r="AH27" s="3"/>
       <c r="AJ27" s="2"/>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -23715,7 +24029,7 @@
       <c r="AH28" s="3"/>
       <c r="AJ28" s="2"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -23765,7 +24079,7 @@
       <c r="AH29" s="3"/>
       <c r="AJ29" s="2"/>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -23815,7 +24129,7 @@
       <c r="AH30" s="3"/>
       <c r="AJ30" s="2"/>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -23865,7 +24179,7 @@
       <c r="AH31" s="3"/>
       <c r="AJ31" s="2"/>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>31</v>
       </c>
@@ -23915,7 +24229,7 @@
       <c r="AH32" s="3"/>
       <c r="AJ32" s="2"/>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -23966,7 +24280,7 @@
       <c r="AH33" s="3"/>
       <c r="AJ33" s="2"/>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -24016,7 +24330,7 @@
       <c r="AH34" s="3"/>
       <c r="AJ34" s="2"/>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>34</v>
       </c>
@@ -24066,7 +24380,7 @@
       <c r="AH35" s="3"/>
       <c r="AJ35" s="2"/>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -24116,7 +24430,7 @@
       <c r="AH36" s="3"/>
       <c r="AJ36" s="2"/>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -24166,7 +24480,7 @@
       <c r="AH37" s="3"/>
       <c r="AJ37" s="2"/>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>37</v>
       </c>
@@ -24216,7 +24530,7 @@
       <c r="AH38" s="3"/>
       <c r="AJ38" s="2"/>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>38</v>
       </c>
@@ -24266,7 +24580,7 @@
       <c r="AH39" s="3"/>
       <c r="AJ39" s="2"/>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -24323,7 +24637,7 @@
       <c r="AH40" s="3"/>
       <c r="AJ40" s="2"/>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>40</v>
       </c>
@@ -24380,7 +24694,7 @@
       <c r="AH41" s="3"/>
       <c r="AJ41" s="2"/>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -24437,7 +24751,7 @@
       <c r="AH42" s="3"/>
       <c r="AJ42" s="2"/>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -24494,7 +24808,7 @@
       <c r="AH43" s="3"/>
       <c r="AJ43" s="2"/>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>43</v>
       </c>
@@ -24551,7 +24865,7 @@
       <c r="AH44" s="3"/>
       <c r="AJ44" s="2"/>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>44</v>
       </c>
@@ -24608,7 +24922,7 @@
       <c r="AH45" s="3"/>
       <c r="AJ45" s="2"/>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -24670,7 +24984,7 @@
       <c r="AH46" s="3"/>
       <c r="AJ46" s="2"/>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -24733,7 +25047,7 @@
       <c r="AH47" s="3"/>
       <c r="AJ47" s="2"/>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>47</v>
       </c>
@@ -24786,7 +25100,7 @@
         <v>293.82901866345577</v>
       </c>
       <c r="N48">
-        <f>Sheet1!H48</f>
+        <f>Sheet1!H49</f>
         <v>143025</v>
       </c>
       <c r="O48">
@@ -24797,7 +25111,7 @@
       <c r="AH48" s="3"/>
       <c r="AJ48" s="2"/>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -24850,7 +25164,7 @@
         <v>333.2480433473811</v>
       </c>
       <c r="N49">
-        <f>Sheet1!H49</f>
+        <f>Sheet1!H50</f>
         <v>163539</v>
       </c>
       <c r="O49">
@@ -24861,7 +25175,7 @@
       <c r="AH49" s="3"/>
       <c r="AJ49" s="2"/>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -24914,7 +25228,7 @@
         <v>378.53702588801929</v>
       </c>
       <c r="N50">
-        <f>Sheet1!H50</f>
+        <f>Sheet1!H51</f>
         <v>186101</v>
       </c>
       <c r="O50">
@@ -24925,7 +25239,7 @@
       <c r="AH50" s="3"/>
       <c r="AJ50" s="2"/>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>50</v>
       </c>
@@ -24977,19 +25291,19 @@
         <f t="shared" si="5"/>
         <v>443.61830222757379</v>
       </c>
-      <c r="N51">
-        <f>Sheet1!H51</f>
-        <v>213144</v>
-      </c>
-      <c r="O51">
+      <c r="N51" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O51" t="e">
         <f t="shared" si="6"/>
-        <v>651.41809290953552</v>
+        <v>#REF!</v>
       </c>
       <c r="AG51" s="2"/>
       <c r="AH51" s="3"/>
       <c r="AJ51" s="2"/>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>51</v>
       </c>
@@ -25003,11 +25317,11 @@
       </c>
       <c r="D52">
         <f>Sheet1!C52</f>
-        <v>0</v>
+        <v>13614</v>
       </c>
       <c r="E52">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>792.43306169965081</v>
       </c>
       <c r="F52">
         <f>Sheet1!D52</f>
@@ -25019,11 +25333,11 @@
       </c>
       <c r="H52">
         <f>Sheet1!E52</f>
-        <v>0</v>
+        <v>73522</v>
       </c>
       <c r="I52">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>888.05411281555735</v>
       </c>
       <c r="J52">
         <f>Sheet1!F52</f>
@@ -25043,16 +25357,16 @@
       </c>
       <c r="N52">
         <f>Sheet1!H52</f>
-        <v>0</v>
+        <v>213144</v>
       </c>
       <c r="O52">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>651.41809290953552</v>
       </c>
       <c r="AG52" s="2"/>
       <c r="AH52" s="3"/>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>52</v>
       </c>
@@ -25066,96 +25380,96 @@
       </c>
       <c r="D53">
         <f>Sheet1!C53</f>
-        <v>0</v>
+        <v>15723</v>
       </c>
       <c r="F53">
         <f>Sheet1!D53</f>
-        <v>0</v>
-      </c>
-      <c r="H53">
+        <v>119827</v>
+      </c>
+      <c r="H53" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J53">
         <f>Sheet1!E53</f>
-        <v>0</v>
-      </c>
-      <c r="J53">
-        <f>Sheet1!F53</f>
-        <v>0</v>
+        <v>79696</v>
       </c>
       <c r="L53">
         <f>Sheet1!G53</f>
-        <v>0</v>
+        <v>38168</v>
       </c>
       <c r="N53">
         <f>Sheet1!H53</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+        <v>239279</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>53</v>
       </c>
       <c r="B54">
         <f>Sheet1!B54</f>
-        <v>0</v>
+        <v>124736</v>
       </c>
       <c r="D54">
         <f>Sheet1!C54</f>
-        <v>0</v>
-      </c>
-      <c r="F54">
-        <f>Sheet1!D54</f>
-        <v>0</v>
-      </c>
-      <c r="H54">
-        <f>Sheet1!E54</f>
-        <v>0</v>
-      </c>
-      <c r="J54">
-        <f>Sheet1!F54</f>
-        <v>0</v>
-      </c>
-      <c r="L54">
-        <f>Sheet1!G54</f>
-        <v>0</v>
+        <v>16627</v>
+      </c>
+      <c r="F54" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H54" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J54" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L54" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="N54">
         <f>Sheet1!H54</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
+        <v>277205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>54</v>
       </c>
       <c r="B55">
         <f>Sheet1!B55</f>
-        <v>0</v>
+        <v>130759</v>
       </c>
       <c r="D55">
         <f>Sheet1!C55</f>
         <v>0</v>
       </c>
       <c r="F55">
-        <f>Sheet1!D55</f>
-        <v>0</v>
+        <f>Sheet1!D54</f>
+        <v>124632</v>
       </c>
       <c r="H55">
-        <f>Sheet1!E55</f>
-        <v>0</v>
+        <f>Sheet1!E54</f>
+        <v>85778</v>
       </c>
       <c r="J55">
-        <f>Sheet1!F55</f>
-        <v>0</v>
+        <f>Sheet1!F54</f>
+        <v>68605</v>
       </c>
       <c r="L55">
-        <f>Sheet1!G55</f>
-        <v>0</v>
+        <f>Sheet1!G54</f>
+        <v>41903</v>
       </c>
       <c r="N55">
         <f>Sheet1!H55</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>55</v>
       </c>
@@ -25188,7 +25502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>56</v>
       </c>
@@ -25221,7 +25535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>57</v>
       </c>
@@ -25254,7 +25568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>58</v>
       </c>
@@ -25287,7 +25601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>59</v>
       </c>
@@ -25320,7 +25634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>60</v>
       </c>
@@ -25353,7 +25667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>61</v>
       </c>
@@ -25386,7 +25700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>62</v>
       </c>
@@ -25419,7 +25733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>63</v>
       </c>
@@ -25452,7 +25766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>64</v>
       </c>
@@ -25485,7 +25799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>65</v>
       </c>
@@ -25518,7 +25832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>66</v>
       </c>
@@ -25551,7 +25865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>67</v>
       </c>
@@ -25584,7 +25898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>68</v>
       </c>
@@ -25617,7 +25931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>69</v>
       </c>
@@ -25657,24 +25971,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AJ70"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="76" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O51" sqref="O51:O52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>43</v>
       </c>
@@ -25700,7 +26014,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -25747,7 +26061,7 @@
         <v>0.12040939193257075</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -25796,7 +26110,7 @@
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -25845,7 +26159,7 @@
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -25894,7 +26208,7 @@
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -25943,7 +26257,7 @@
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -25993,7 +26307,7 @@
       <c r="AH7" s="2"/>
       <c r="AJ7" s="2"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -26043,7 +26357,7 @@
       <c r="AH8" s="2"/>
       <c r="AJ8" s="2"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -26093,7 +26407,7 @@
       <c r="AH9" s="2"/>
       <c r="AJ9" s="2"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -26143,7 +26457,7 @@
       <c r="AH10" s="2"/>
       <c r="AJ10" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -26191,7 +26505,7 @@
       </c>
       <c r="AJ11" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -26239,7 +26553,7 @@
       </c>
       <c r="AJ12" s="2"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -26287,7 +26601,7 @@
       </c>
       <c r="AJ13" s="2"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -26335,7 +26649,7 @@
       </c>
       <c r="AJ14" s="2"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -26383,7 +26697,7 @@
       </c>
       <c r="AJ15" s="2"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -26431,7 +26745,7 @@
       </c>
       <c r="AJ16" s="2"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -26479,7 +26793,7 @@
       </c>
       <c r="AJ17" s="2"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -26527,7 +26841,7 @@
       </c>
       <c r="AJ18" s="2"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -26568,7 +26882,7 @@
       </c>
       <c r="AJ19" s="2"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -26611,7 +26925,7 @@
       <c r="AH20" s="2"/>
       <c r="AJ20" s="2"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -26661,7 +26975,7 @@
       <c r="AH21" s="3"/>
       <c r="AJ21" s="2"/>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -26711,7 +27025,7 @@
       <c r="AH22" s="3"/>
       <c r="AJ22" s="2"/>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -26761,7 +27075,7 @@
       <c r="AH23" s="3"/>
       <c r="AJ23" s="2"/>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -26811,7 +27125,7 @@
       <c r="AH24" s="3"/>
       <c r="AJ24" s="2"/>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -26862,7 +27176,7 @@
       <c r="AH25" s="3"/>
       <c r="AJ25" s="2"/>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -26905,7 +27219,7 @@
       <c r="AH26" s="3"/>
       <c r="AJ26" s="2"/>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -26949,7 +27263,7 @@
       <c r="AH27" s="3"/>
       <c r="AJ27" s="2"/>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -26999,7 +27313,7 @@
       <c r="AH28" s="3"/>
       <c r="AJ28" s="2"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -27049,7 +27363,7 @@
       <c r="AH29" s="3"/>
       <c r="AJ29" s="2"/>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -27099,7 +27413,7 @@
       <c r="AH30" s="3"/>
       <c r="AJ30" s="2"/>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -27149,7 +27463,7 @@
       <c r="AH31" s="3"/>
       <c r="AJ31" s="2"/>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>31</v>
       </c>
@@ -27199,7 +27513,7 @@
       <c r="AH32" s="3"/>
       <c r="AJ32" s="2"/>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -27250,7 +27564,7 @@
       <c r="AH33" s="3"/>
       <c r="AJ33" s="2"/>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -27300,7 +27614,7 @@
       <c r="AH34" s="3"/>
       <c r="AJ34" s="2"/>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>34</v>
       </c>
@@ -27350,7 +27664,7 @@
       <c r="AH35" s="3"/>
       <c r="AJ35" s="2"/>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -27400,7 +27714,7 @@
       <c r="AH36" s="3"/>
       <c r="AJ36" s="2"/>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -27450,7 +27764,7 @@
       <c r="AH37" s="3"/>
       <c r="AJ37" s="2"/>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>37</v>
       </c>
@@ -27500,7 +27814,7 @@
       <c r="AH38" s="3"/>
       <c r="AJ38" s="2"/>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>38</v>
       </c>
@@ -27550,7 +27864,7 @@
       <c r="AH39" s="3"/>
       <c r="AJ39" s="2"/>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -27607,7 +27921,7 @@
       <c r="AH40" s="3"/>
       <c r="AJ40" s="2"/>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>40</v>
       </c>
@@ -27664,7 +27978,7 @@
       <c r="AH41" s="3"/>
       <c r="AJ41" s="2"/>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -27721,7 +28035,7 @@
       <c r="AH42" s="3"/>
       <c r="AJ42" s="2"/>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -27778,7 +28092,7 @@
       <c r="AH43" s="3"/>
       <c r="AJ43" s="2"/>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>43</v>
       </c>
@@ -27835,7 +28149,7 @@
       <c r="AH44" s="3"/>
       <c r="AJ44" s="2"/>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>44</v>
       </c>
@@ -27892,7 +28206,7 @@
       <c r="AH45" s="3"/>
       <c r="AJ45" s="2"/>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -27954,7 +28268,7 @@
       <c r="AH46" s="3"/>
       <c r="AJ46" s="2"/>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -28017,7 +28331,7 @@
       <c r="AH47" s="3"/>
       <c r="AJ47" s="2"/>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>47</v>
       </c>
@@ -28070,7 +28384,7 @@
         <v>293.82901866345577</v>
       </c>
       <c r="N48">
-        <f>Sheet1!H48</f>
+        <f>Sheet1!H49</f>
         <v>143025</v>
       </c>
       <c r="O48">
@@ -28081,7 +28395,7 @@
       <c r="AH48" s="3"/>
       <c r="AJ48" s="2"/>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -28134,7 +28448,7 @@
         <v>333.2480433473811</v>
       </c>
       <c r="N49">
-        <f>Sheet1!H49</f>
+        <f>Sheet1!H50</f>
         <v>163539</v>
       </c>
       <c r="O49">
@@ -28145,7 +28459,7 @@
       <c r="AH49" s="3"/>
       <c r="AJ49" s="2"/>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -28198,7 +28512,7 @@
         <v>378.53702588801929</v>
       </c>
       <c r="N50">
-        <f>Sheet1!H50</f>
+        <f>Sheet1!H51</f>
         <v>186101</v>
       </c>
       <c r="O50">
@@ -28209,7 +28523,7 @@
       <c r="AH50" s="3"/>
       <c r="AJ50" s="2"/>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>50</v>
       </c>
@@ -28261,19 +28575,19 @@
         <f t="shared" si="5"/>
         <v>443.61830222757379</v>
       </c>
-      <c r="N51">
-        <f>Sheet1!H51</f>
-        <v>213144</v>
-      </c>
-      <c r="O51">
+      <c r="N51" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O51" t="e">
         <f t="shared" si="6"/>
-        <v>651.41809290953552</v>
+        <v>#REF!</v>
       </c>
       <c r="AG51" s="2"/>
       <c r="AH51" s="3"/>
       <c r="AJ51" s="2"/>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>51</v>
       </c>
@@ -28287,11 +28601,11 @@
       </c>
       <c r="D52">
         <f>Sheet1!C52</f>
-        <v>0</v>
+        <v>13614</v>
       </c>
       <c r="E52">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>792.43306169965081</v>
       </c>
       <c r="F52">
         <f>Sheet1!D52</f>
@@ -28303,11 +28617,11 @@
       </c>
       <c r="H52">
         <f>Sheet1!E52</f>
-        <v>0</v>
+        <v>73522</v>
       </c>
       <c r="I52">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>888.05411281555735</v>
       </c>
       <c r="J52">
         <f>Sheet1!F52</f>
@@ -28327,16 +28641,16 @@
       </c>
       <c r="N52">
         <f>Sheet1!H52</f>
-        <v>0</v>
+        <v>213144</v>
       </c>
       <c r="O52">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>651.41809290953552</v>
       </c>
       <c r="AG52" s="2"/>
       <c r="AH52" s="3"/>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>52</v>
       </c>
@@ -28350,96 +28664,96 @@
       </c>
       <c r="D53">
         <f>Sheet1!C53</f>
-        <v>0</v>
+        <v>15723</v>
       </c>
       <c r="F53">
         <f>Sheet1!D53</f>
-        <v>0</v>
-      </c>
-      <c r="H53">
+        <v>119827</v>
+      </c>
+      <c r="H53" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J53">
         <f>Sheet1!E53</f>
-        <v>0</v>
-      </c>
-      <c r="J53">
-        <f>Sheet1!F53</f>
-        <v>0</v>
+        <v>79696</v>
       </c>
       <c r="L53">
         <f>Sheet1!G53</f>
-        <v>0</v>
+        <v>38168</v>
       </c>
       <c r="N53">
         <f>Sheet1!H53</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+        <v>239279</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>53</v>
       </c>
       <c r="B54">
         <f>Sheet1!B54</f>
-        <v>0</v>
+        <v>124736</v>
       </c>
       <c r="D54">
         <f>Sheet1!C54</f>
-        <v>0</v>
-      </c>
-      <c r="F54">
-        <f>Sheet1!D54</f>
-        <v>0</v>
-      </c>
-      <c r="H54">
-        <f>Sheet1!E54</f>
-        <v>0</v>
-      </c>
-      <c r="J54">
-        <f>Sheet1!F54</f>
-        <v>0</v>
-      </c>
-      <c r="L54">
-        <f>Sheet1!G54</f>
-        <v>0</v>
+        <v>16627</v>
+      </c>
+      <c r="F54" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H54" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J54" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L54" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="N54">
         <f>Sheet1!H54</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
+        <v>277205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>54</v>
       </c>
       <c r="B55">
         <f>Sheet1!B55</f>
-        <v>0</v>
+        <v>130759</v>
       </c>
       <c r="D55">
         <f>Sheet1!C55</f>
         <v>0</v>
       </c>
       <c r="F55">
-        <f>Sheet1!D55</f>
-        <v>0</v>
+        <f>Sheet1!D54</f>
+        <v>124632</v>
       </c>
       <c r="H55">
-        <f>Sheet1!E55</f>
-        <v>0</v>
+        <f>Sheet1!E54</f>
+        <v>85778</v>
       </c>
       <c r="J55">
-        <f>Sheet1!F55</f>
-        <v>0</v>
+        <f>Sheet1!F54</f>
+        <v>68605</v>
       </c>
       <c r="L55">
-        <f>Sheet1!G55</f>
-        <v>0</v>
+        <f>Sheet1!G54</f>
+        <v>41903</v>
       </c>
       <c r="N55">
         <f>Sheet1!H55</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>55</v>
       </c>
@@ -28472,7 +28786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>56</v>
       </c>
@@ -28505,7 +28819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>57</v>
       </c>
@@ -28538,7 +28852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>58</v>
       </c>
@@ -28571,7 +28885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>59</v>
       </c>
@@ -28604,7 +28918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>60</v>
       </c>
@@ -28637,7 +28951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>61</v>
       </c>
@@ -28670,7 +28984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>62</v>
       </c>
@@ -28703,7 +29017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>63</v>
       </c>
@@ -28736,7 +29050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>64</v>
       </c>
@@ -28769,7 +29083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>65</v>
       </c>
@@ -28802,7 +29116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>66</v>
       </c>
@@ -28835,7 +29149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>67</v>
       </c>
@@ -28868,7 +29182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>68</v>
       </c>
@@ -28901,7 +29215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
Include Deaths data for other countries
</commit_message>
<xml_diff>
--- a/Sources/Paises.xlsx
+++ b/Sources/Paises.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\PowerBI_Covid\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DAA985-561E-4EBA-9264-951E2BED87A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E510292C-E03A-488F-8AC8-DF8B29D36481}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8250" yWindow="285" windowWidth="20490" windowHeight="15915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="MP100pmillon" sheetId="4" r:id="rId3"/>
-    <sheet name="MP200pmillon" sheetId="3" r:id="rId4"/>
-    <sheet name="MP500pmillon" sheetId="5" r:id="rId5"/>
+    <sheet name="Casos" sheetId="1" r:id="rId1"/>
+    <sheet name="Fallecidos" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="MP100pmillon" sheetId="4" r:id="rId4"/>
+    <sheet name="MP200pmillon" sheetId="3" r:id="rId5"/>
+    <sheet name="MP500pmillon" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
   <si>
     <t>Italia</t>
   </si>
@@ -307,7 +308,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Casos!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -352,7 +353,7 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$8:$A$69</c:f>
+              <c:f>Casos!$A$8:$A$69</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="62"/>
@@ -547,7 +548,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$63</c:f>
+              <c:f>Casos!$B$2:$B$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="62"/>
@@ -731,7 +732,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Casos!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -754,7 +755,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$70</c:f>
+              <c:f>Casos!$A$2:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="69"/>
@@ -970,7 +971,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$70</c:f>
+              <c:f>Casos!$C$2:$C$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="69"/>
@@ -1166,7 +1167,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Casos!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1211,7 +1212,7 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$70</c:f>
+              <c:f>Casos!$A$17:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="54"/>
@@ -1382,7 +1383,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$54</c:f>
+              <c:f>Casos!$D$2:$D$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="53"/>
@@ -1560,7 +1561,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Casos!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1583,7 +1584,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$69</c:f>
+              <c:f>Casos!$A$7:$A$69</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="63"/>
@@ -1781,7 +1782,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$63</c:f>
+              <c:f>Casos!$E$2:$E$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="62"/>
@@ -1977,7 +1978,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>Casos!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2022,7 +2023,7 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$8:$A$70</c:f>
+              <c:f>Casos!$A$8:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="63"/>
@@ -2220,7 +2221,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$64</c:f>
+              <c:f>Casos!$F$2:$F$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="63"/>
@@ -2416,7 +2417,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Casos!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2439,7 +2440,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$70</c:f>
+              <c:f>Casos!$A$2:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="69"/>
@@ -2655,7 +2656,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$70</c:f>
+              <c:f>Casos!$G$2:$G$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="69"/>
@@ -2851,7 +2852,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>Casos!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2876,7 +2877,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$51:$A$115</c:f>
+              <c:f>Casos!$A$51:$A$115</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="65"/>
@@ -2945,7 +2946,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$41:$H$48</c:f>
+              <c:f>Casos!$H$41:$H$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3284,7 +3285,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$AL$14:$AL$36</c:f>
+              <c:f>Casos!$AL$14:$AL$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
@@ -3362,7 +3363,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$AG$14:$AG$36</c:f>
+              <c:f>Casos!$AG$14:$AG$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
@@ -15754,8 +15755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AC44" sqref="AC44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18176,11 +18177,11 @@
         <v>3.8311025408348458E-2</v>
       </c>
       <c r="AA40" s="3">
-        <f t="shared" ref="AA40:AA41" si="31">Y40-Y39</f>
+        <f t="shared" ref="AA40" si="31">Y40-Y39</f>
         <v>4053</v>
       </c>
       <c r="AB40" s="3">
-        <f t="shared" ref="AB40:AB41" si="32">SUM(AA37:AA40)</f>
+        <f t="shared" ref="AB40" si="32">SUM(AA37:AA40)</f>
         <v>19294</v>
       </c>
       <c r="AD40" s="2" t="e">
@@ -18235,11 +18236,11 @@
         <v>4.3247056270009222E-2</v>
       </c>
       <c r="AA41" s="3">
-        <f t="shared" si="31"/>
+        <f>Y41-Y40</f>
         <v>4782</v>
       </c>
       <c r="AB41" s="3">
-        <f t="shared" si="32"/>
+        <f>SUM(AA38:AA41)</f>
         <v>18102</v>
       </c>
       <c r="AD41" s="2" t="e">
@@ -18819,6 +18820,1072 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C86610-CB55-4FA2-9727-343B46DC10BB}">
+  <dimension ref="A1:H70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43873</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43874</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43876</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43877</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43878</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43881</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43882</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43883</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43884</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43885</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43886</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43887</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43888</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>12</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43889</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43890</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>12</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43891</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>17</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43892</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>34</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43893</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>52</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43894</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>80</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43895</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>107</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>43896</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>148</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43897</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>148</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43898</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>148</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43899</v>
+      </c>
+      <c r="B28">
+        <v>28</v>
+      </c>
+      <c r="D28">
+        <v>366</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43900</v>
+      </c>
+      <c r="B29">
+        <v>36</v>
+      </c>
+      <c r="D29">
+        <v>463</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43901</v>
+      </c>
+      <c r="B30">
+        <v>48</v>
+      </c>
+      <c r="D30">
+        <v>631</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43902</v>
+      </c>
+      <c r="B31">
+        <v>84</v>
+      </c>
+      <c r="D31">
+        <v>827</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>43903</v>
+      </c>
+      <c r="B32">
+        <v>120</v>
+      </c>
+      <c r="D32">
+        <v>1016</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>43904</v>
+      </c>
+      <c r="B33">
+        <v>134</v>
+      </c>
+      <c r="D33">
+        <v>1266</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>43905</v>
+      </c>
+      <c r="B34">
+        <v>285</v>
+      </c>
+      <c r="D34">
+        <v>1441</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
+      </c>
+      <c r="F34">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>43906</v>
+      </c>
+      <c r="B35">
+        <v>306</v>
+      </c>
+      <c r="D35">
+        <v>1809</v>
+      </c>
+      <c r="E35">
+        <v>12</v>
+      </c>
+      <c r="F35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>43907</v>
+      </c>
+      <c r="B36">
+        <v>491</v>
+      </c>
+      <c r="D36">
+        <v>1809</v>
+      </c>
+      <c r="E36">
+        <v>12</v>
+      </c>
+      <c r="F36">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>43908</v>
+      </c>
+      <c r="B37">
+        <v>598</v>
+      </c>
+      <c r="D37">
+        <v>1809</v>
+      </c>
+      <c r="E37">
+        <v>12</v>
+      </c>
+      <c r="F37">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>43909</v>
+      </c>
+      <c r="B38">
+        <v>767</v>
+      </c>
+      <c r="D38">
+        <v>2978</v>
+      </c>
+      <c r="E38">
+        <v>12</v>
+      </c>
+      <c r="F38">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>43910</v>
+      </c>
+      <c r="B39">
+        <v>982</v>
+      </c>
+      <c r="D39">
+        <v>3405</v>
+      </c>
+      <c r="E39">
+        <v>20</v>
+      </c>
+      <c r="F39">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>43911</v>
+      </c>
+      <c r="B40">
+        <v>1326</v>
+      </c>
+      <c r="D40">
+        <v>4032</v>
+      </c>
+      <c r="E40">
+        <v>31</v>
+      </c>
+      <c r="F40">
+        <v>450</v>
+      </c>
+      <c r="H40">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B41">
+        <v>1720</v>
+      </c>
+      <c r="D41">
+        <v>4825</v>
+      </c>
+      <c r="E41">
+        <v>46</v>
+      </c>
+      <c r="F41">
+        <v>562</v>
+      </c>
+      <c r="H41">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B42">
+        <v>2182</v>
+      </c>
+      <c r="D42">
+        <v>5476</v>
+      </c>
+      <c r="E42">
+        <v>55</v>
+      </c>
+      <c r="F42">
+        <v>674</v>
+      </c>
+      <c r="H42">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B43">
+        <v>2696</v>
+      </c>
+      <c r="D43">
+        <v>6077</v>
+      </c>
+      <c r="E43">
+        <v>86</v>
+      </c>
+      <c r="F43">
+        <v>860</v>
+      </c>
+      <c r="G43">
+        <v>335</v>
+      </c>
+      <c r="H43">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B44">
+        <v>3434</v>
+      </c>
+      <c r="D44">
+        <v>6820</v>
+      </c>
+      <c r="E44">
+        <v>114</v>
+      </c>
+      <c r="F44">
+        <v>1100</v>
+      </c>
+      <c r="G44">
+        <v>442</v>
+      </c>
+      <c r="H44">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43916</v>
+      </c>
+      <c r="B45">
+        <v>4089</v>
+      </c>
+      <c r="D45">
+        <v>7503</v>
+      </c>
+      <c r="E45">
+        <v>149</v>
+      </c>
+      <c r="F45">
+        <v>1331</v>
+      </c>
+      <c r="G45">
+        <v>422</v>
+      </c>
+      <c r="H45">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B46">
+        <v>4858</v>
+      </c>
+      <c r="D46">
+        <v>8165</v>
+      </c>
+      <c r="E46">
+        <v>198</v>
+      </c>
+      <c r="F46">
+        <v>1686</v>
+      </c>
+      <c r="G46">
+        <v>578</v>
+      </c>
+      <c r="H46">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43918</v>
+      </c>
+      <c r="B47">
+        <v>5710</v>
+      </c>
+      <c r="D47">
+        <v>9134</v>
+      </c>
+      <c r="E47">
+        <v>253</v>
+      </c>
+      <c r="F47">
+        <v>1995</v>
+      </c>
+      <c r="G47">
+        <v>759</v>
+      </c>
+      <c r="H47">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B48">
+        <v>6528</v>
+      </c>
+      <c r="D48">
+        <v>10023</v>
+      </c>
+      <c r="E48">
+        <v>325</v>
+      </c>
+      <c r="F48">
+        <v>2314</v>
+      </c>
+      <c r="G48">
+        <v>1019</v>
+      </c>
+      <c r="H48">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B49">
+        <v>7340</v>
+      </c>
+      <c r="D49">
+        <v>10779</v>
+      </c>
+      <c r="E49">
+        <v>389</v>
+      </c>
+      <c r="F49">
+        <v>2606</v>
+      </c>
+      <c r="G49">
+        <v>1228</v>
+      </c>
+      <c r="H49">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>43921</v>
+      </c>
+      <c r="B50">
+        <v>8189</v>
+      </c>
+      <c r="D50">
+        <v>11591</v>
+      </c>
+      <c r="E50">
+        <v>455</v>
+      </c>
+      <c r="F50">
+        <v>3025</v>
+      </c>
+      <c r="G50">
+        <v>1408</v>
+      </c>
+      <c r="H50">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B51">
+        <v>9053</v>
+      </c>
+      <c r="D51">
+        <v>12428</v>
+      </c>
+      <c r="E51">
+        <v>583</v>
+      </c>
+      <c r="F51">
+        <v>3523</v>
+      </c>
+      <c r="G51">
+        <v>1789</v>
+      </c>
+      <c r="H51">
+        <v>2860</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B52">
+        <v>10003</v>
+      </c>
+      <c r="D52">
+        <v>13155</v>
+      </c>
+      <c r="E52">
+        <v>732</v>
+      </c>
+      <c r="F52">
+        <v>4032</v>
+      </c>
+      <c r="G52">
+        <v>2352</v>
+      </c>
+      <c r="H52">
+        <v>3603</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>43924</v>
+      </c>
+      <c r="B53">
+        <v>10935</v>
+      </c>
+      <c r="D53">
+        <v>13915</v>
+      </c>
+      <c r="E53">
+        <v>872</v>
+      </c>
+      <c r="F53">
+        <v>4503</v>
+      </c>
+      <c r="G53">
+        <v>2921</v>
+      </c>
+      <c r="H53">
+        <v>4513</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>43925</v>
+      </c>
+      <c r="B54">
+        <v>11744</v>
+      </c>
+      <c r="C54">
+        <v>1487</v>
+      </c>
+      <c r="D54">
+        <v>14681</v>
+      </c>
+      <c r="E54">
+        <v>1017</v>
+      </c>
+      <c r="F54">
+        <v>6507</v>
+      </c>
+      <c r="G54">
+        <v>3605</v>
+      </c>
+      <c r="H54">
+        <v>5443</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>43926</v>
+      </c>
+      <c r="B55">
+        <v>12418</v>
+      </c>
+      <c r="C55">
+        <v>1651</v>
+      </c>
+      <c r="D55">
+        <v>15362</v>
+      </c>
+      <c r="E55">
+        <v>1158</v>
+      </c>
+      <c r="F55">
+        <v>7560</v>
+      </c>
+      <c r="G55">
+        <v>4313</v>
+      </c>
+      <c r="H55">
+        <v>6593</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B56">
+        <v>13055</v>
+      </c>
+      <c r="C56">
+        <v>1766</v>
+      </c>
+      <c r="D56">
+        <v>15887</v>
+      </c>
+      <c r="E56">
+        <v>1342</v>
+      </c>
+      <c r="F56">
+        <v>8078</v>
+      </c>
+      <c r="G56">
+        <v>4934</v>
+      </c>
+      <c r="H56">
+        <v>7616</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B57">
+        <v>13798</v>
+      </c>
+      <c r="C57">
+        <v>1867</v>
+      </c>
+      <c r="D57">
+        <v>16523</v>
+      </c>
+      <c r="E57">
+        <v>1434</v>
+      </c>
+      <c r="F57">
+        <v>8911</v>
+      </c>
+      <c r="G57">
+        <v>5373</v>
+      </c>
+      <c r="H57">
+        <v>8910</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>43929</v>
+      </c>
+      <c r="B58">
+        <v>14555</v>
+      </c>
+      <c r="C58">
+        <v>2101</v>
+      </c>
+      <c r="D58">
+        <v>17127</v>
+      </c>
+      <c r="E58">
+        <v>1607</v>
+      </c>
+      <c r="F58">
+        <v>10328</v>
+      </c>
+      <c r="G58">
+        <v>6159</v>
+      </c>
+      <c r="H58">
+        <v>12064</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B59">
+        <v>15238</v>
+      </c>
+      <c r="C59">
+        <v>2248</v>
+      </c>
+      <c r="D59">
+        <v>17669</v>
+      </c>
+      <c r="E59">
+        <v>1861</v>
+      </c>
+      <c r="F59">
+        <v>10869</v>
+      </c>
+      <c r="G59">
+        <v>7097</v>
+      </c>
+      <c r="H59">
+        <v>12754</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>43931</v>
+      </c>
+      <c r="B60">
+        <v>15843</v>
+      </c>
+      <c r="C60">
+        <v>2396</v>
+      </c>
+      <c r="D60">
+        <v>18279</v>
+      </c>
+      <c r="E60">
+        <v>2107</v>
+      </c>
+      <c r="F60">
+        <v>12210</v>
+      </c>
+      <c r="G60">
+        <v>7978</v>
+      </c>
+      <c r="H60">
+        <v>14696</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>43932</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>43933</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>43934</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>43935</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>43937</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>43938</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>43939</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>43940</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>43941</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y14"/>
   <sheetViews>
@@ -19548,7 +20615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ70"/>
   <sheetViews>
@@ -21796,7 +22863,7 @@
         <v>1372.8889841405917</v>
       </c>
       <c r="D46">
-        <f>Sheet1!C46</f>
+        <f>Casos!C46</f>
         <v>8603</v>
       </c>
       <c r="E46">
@@ -21804,7 +22871,7 @@
         <v>500.75669383003492</v>
       </c>
       <c r="F46">
-        <f>Sheet1!D46</f>
+        <f>Casos!D46</f>
         <v>86498</v>
       </c>
       <c r="G46">
@@ -21812,7 +22879,7 @@
         <v>1430.1917989417991</v>
       </c>
       <c r="H46">
-        <f>Sheet1!E46</f>
+        <f>Casos!E46</f>
         <v>48582</v>
       </c>
       <c r="I46">
@@ -21820,7 +22887,7 @@
         <v>586.8100012078753</v>
       </c>
       <c r="J46">
-        <f>Sheet1!F46</f>
+        <f>Casos!F46</f>
         <v>32964</v>
       </c>
       <c r="K46">
@@ -21828,7 +22895,7 @@
         <v>492.07344379758177</v>
       </c>
       <c r="L46">
-        <f>Sheet1!G46</f>
+        <f>Casos!G46</f>
         <v>14543</v>
       </c>
       <c r="M46">
@@ -21851,7 +22918,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <f>Sheet1!B47</f>
+        <f>Casos!B47</f>
         <v>72248</v>
       </c>
       <c r="C47">
@@ -21859,7 +22926,7 @@
         <v>1548.3926275182171</v>
       </c>
       <c r="D47">
-        <f>Sheet1!C47</f>
+        <f>Casos!C47</f>
         <v>9762</v>
       </c>
       <c r="E47">
@@ -21867,7 +22934,7 @@
         <v>568.21885913853316</v>
       </c>
       <c r="F47">
-        <f>Sheet1!D47</f>
+        <f>Casos!D47</f>
         <v>92472</v>
       </c>
       <c r="G47">
@@ -21875,7 +22942,7 @@
         <v>1528.968253968254</v>
       </c>
       <c r="H47">
-        <f>Sheet1!E47</f>
+        <f>Casos!E47</f>
         <v>52547</v>
       </c>
       <c r="I47">
@@ -21883,7 +22950,7 @@
         <v>634.70225872689934</v>
       </c>
       <c r="J47">
-        <f>Sheet1!F47</f>
+        <f>Casos!F47</f>
         <v>37575</v>
       </c>
       <c r="K47">
@@ -21891,7 +22958,7 @@
         <v>560.90461262875056</v>
       </c>
       <c r="L47">
-        <f>Sheet1!G47</f>
+        <f>Casos!G47</f>
         <v>17089</v>
       </c>
       <c r="M47">
@@ -21914,7 +22981,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <f>Sheet1!B48</f>
+        <f>Casos!B48</f>
         <v>78797</v>
       </c>
       <c r="C48">
@@ -21922,7 +22989,7 @@
         <v>1688.7483926275183</v>
       </c>
       <c r="D48">
-        <f>Sheet1!C48</f>
+        <f>Casos!C48</f>
         <v>10866</v>
       </c>
       <c r="E48">
@@ -21930,7 +22997,7 @@
         <v>632.47962747380677</v>
       </c>
       <c r="F48">
-        <f>Sheet1!D48</f>
+        <f>Casos!D48</f>
         <v>97689</v>
       </c>
       <c r="G48">
@@ -21938,7 +23005,7 @@
         <v>1615.2281746031747</v>
       </c>
       <c r="H48">
-        <f>Sheet1!E48</f>
+        <f>Casos!E48</f>
         <v>57298</v>
       </c>
       <c r="I48">
@@ -21946,7 +23013,7 @@
         <v>692.08841647541965</v>
       </c>
       <c r="J48">
-        <f>Sheet1!F48</f>
+        <f>Casos!F48</f>
         <v>40174</v>
       </c>
       <c r="K48">
@@ -21954,7 +23021,7 @@
         <v>599.70144797731007</v>
       </c>
       <c r="L48">
-        <f>Sheet1!G48</f>
+        <f>Casos!G48</f>
         <v>19522</v>
       </c>
       <c r="M48">
@@ -21962,7 +23029,7 @@
         <v>293.82901866345577</v>
       </c>
       <c r="N48">
-        <f>Sheet1!H49</f>
+        <f>Casos!H49</f>
         <v>143025</v>
       </c>
       <c r="O48">
@@ -21978,7 +23045,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <f>Sheet1!B49</f>
+        <f>Casos!B49</f>
         <v>85195</v>
       </c>
       <c r="C49">
@@ -21986,7 +23053,7 @@
         <v>1825.867981140163</v>
       </c>
       <c r="D49">
-        <f>Sheet1!C49</f>
+        <f>Casos!C49</f>
         <v>11750</v>
       </c>
       <c r="E49">
@@ -21994,7 +23061,7 @@
         <v>683.93480791618163</v>
       </c>
       <c r="F49">
-        <f>Sheet1!D49</f>
+        <f>Casos!D49</f>
         <v>101739</v>
       </c>
       <c r="G49">
@@ -22002,7 +23069,7 @@
         <v>1682.1924603174605</v>
       </c>
       <c r="H49">
-        <f>Sheet1!E49</f>
+        <f>Casos!E49</f>
         <v>61913</v>
       </c>
       <c r="I49">
@@ -22010,7 +23077,7 @@
         <v>747.83186375166076</v>
       </c>
       <c r="J49">
-        <f>Sheet1!F49</f>
+        <f>Casos!F49</f>
         <v>44550</v>
       </c>
       <c r="K49">
@@ -22018,7 +23085,7 @@
         <v>665.02463054187194</v>
       </c>
       <c r="L49">
-        <f>Sheet1!G49</f>
+        <f>Casos!G49</f>
         <v>22141</v>
       </c>
       <c r="M49">
@@ -22026,7 +23093,7 @@
         <v>333.2480433473811</v>
       </c>
       <c r="N49">
-        <f>Sheet1!H50</f>
+        <f>Casos!H50</f>
         <v>163539</v>
       </c>
       <c r="O49">
@@ -22042,7 +23109,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <f>Sheet1!B50</f>
+        <f>Casos!B50</f>
         <v>94417</v>
       </c>
       <c r="C50">
@@ -22050,7 +23117,7 @@
         <v>2023.5105015002146</v>
       </c>
       <c r="D50">
-        <f>Sheet1!C50</f>
+        <f>Casos!C50</f>
         <v>12595</v>
       </c>
       <c r="E50">
@@ -22058,7 +23125,7 @@
         <v>733.11990686845172</v>
       </c>
       <c r="F50">
-        <f>Sheet1!D50</f>
+        <f>Casos!D50</f>
         <v>105792</v>
       </c>
       <c r="G50">
@@ -22066,7 +23133,7 @@
         <v>1749.2063492063494</v>
       </c>
       <c r="H50">
-        <f>Sheet1!E50</f>
+        <f>Casos!E50</f>
         <v>67366</v>
       </c>
       <c r="I50">
@@ -22074,7 +23141,7 @@
         <v>813.6973064379755</v>
       </c>
       <c r="J50">
-        <f>Sheet1!F50</f>
+        <f>Casos!F50</f>
         <v>52128</v>
       </c>
       <c r="K50">
@@ -22082,7 +23149,7 @@
         <v>778.14599193909544</v>
       </c>
       <c r="L50">
-        <f>Sheet1!G50</f>
+        <f>Casos!G50</f>
         <v>25150</v>
       </c>
       <c r="M50">
@@ -22090,7 +23157,7 @@
         <v>378.53702588801929</v>
       </c>
       <c r="N50">
-        <f>Sheet1!H51</f>
+        <f>Casos!H51</f>
         <v>186101</v>
       </c>
       <c r="O50">
@@ -22106,7 +23173,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <f>Sheet1!B51</f>
+        <f>Casos!B51</f>
         <v>102136</v>
       </c>
       <c r="C51">
@@ -22114,7 +23181,7 @@
         <v>2188.9412773253325</v>
       </c>
       <c r="D51">
-        <f>Sheet1!C51</f>
+        <f>Casos!C51</f>
         <v>13614</v>
       </c>
       <c r="E51">
@@ -22122,7 +23189,7 @@
         <v>792.43306169965081</v>
       </c>
       <c r="F51">
-        <f>Sheet1!D51</f>
+        <f>Casos!D51</f>
         <v>110574</v>
       </c>
       <c r="G51">
@@ -22130,7 +23197,7 @@
         <v>1828.2738095238096</v>
       </c>
       <c r="H51">
-        <f>Sheet1!E51</f>
+        <f>Casos!E51</f>
         <v>73522</v>
       </c>
       <c r="I51">
@@ -22138,7 +23205,7 @@
         <v>888.05411281555735</v>
       </c>
       <c r="J51">
-        <f>Sheet1!F51</f>
+        <f>Casos!F51</f>
         <v>56989</v>
       </c>
       <c r="K51">
@@ -22146,7 +23213,7 @@
         <v>850.70906105388872</v>
       </c>
       <c r="L51">
-        <f>Sheet1!G51</f>
+        <f>Casos!G51</f>
         <v>29474</v>
       </c>
       <c r="M51">
@@ -22154,7 +23221,7 @@
         <v>443.61830222757379</v>
       </c>
       <c r="N51" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="O51" t="e">
@@ -22170,7 +23237,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <f>Sheet1!B52</f>
+        <f>Casos!B52</f>
         <v>110238</v>
       </c>
       <c r="C52">
@@ -22178,7 +23245,7 @@
         <v>2362.5803686240893</v>
       </c>
       <c r="D52">
-        <f>Sheet1!C52</f>
+        <f>Casos!C52</f>
         <v>13614</v>
       </c>
       <c r="E52">
@@ -22186,7 +23253,7 @@
         <v>792.43306169965081</v>
       </c>
       <c r="F52">
-        <f>Sheet1!D52</f>
+        <f>Casos!D52</f>
         <v>115242</v>
       </c>
       <c r="G52">
@@ -22194,7 +23261,7 @@
         <v>1905.4563492063494</v>
       </c>
       <c r="H52">
-        <f>Sheet1!E52</f>
+        <f>Casos!E52</f>
         <v>73522</v>
       </c>
       <c r="I52">
@@ -22202,7 +23269,7 @@
         <v>888.05411281555735</v>
       </c>
       <c r="J52">
-        <f>Sheet1!F52</f>
+        <f>Casos!F52</f>
         <v>59105</v>
       </c>
       <c r="K52">
@@ -22210,7 +23277,7 @@
         <v>882.29586505448583</v>
       </c>
       <c r="L52">
-        <f>Sheet1!G52</f>
+        <f>Casos!G52</f>
         <v>33718</v>
       </c>
       <c r="M52">
@@ -22218,7 +23285,7 @@
         <v>507.49548464780253</v>
       </c>
       <c r="N52">
-        <f>Sheet1!H52</f>
+        <f>Casos!H52</f>
         <v>213144</v>
       </c>
       <c r="O52">
@@ -22233,7 +23300,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <f>Sheet1!B53</f>
+        <f>Casos!B53</f>
         <v>117710</v>
       </c>
       <c r="C53">
@@ -22241,27 +23308,27 @@
         <v>2522.717531075868</v>
       </c>
       <c r="D53">
-        <f>Sheet1!C53</f>
+        <f>Casos!C53</f>
         <v>15723</v>
       </c>
       <c r="F53">
-        <f>Sheet1!D53</f>
+        <f>Casos!D53</f>
         <v>119827</v>
       </c>
       <c r="H53" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="J53">
-        <f>Sheet1!E53</f>
+        <f>Casos!E53</f>
         <v>79696</v>
       </c>
       <c r="L53">
-        <f>Sheet1!G53</f>
+        <f>Casos!G53</f>
         <v>38168</v>
       </c>
       <c r="N53">
-        <f>Sheet1!H53</f>
+        <f>Casos!H53</f>
         <v>239279</v>
       </c>
     </row>
@@ -22270,31 +23337,31 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <f>Sheet1!B54</f>
+        <f>Casos!B54</f>
         <v>124736</v>
       </c>
       <c r="D54">
-        <f>Sheet1!C54</f>
+        <f>Casos!C54</f>
         <v>16627</v>
       </c>
       <c r="F54" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="H54" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="J54" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="L54" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="N54">
-        <f>Sheet1!H54</f>
+        <f>Casos!H54</f>
         <v>277205</v>
       </c>
     </row>
@@ -22303,7 +23370,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <f>Sheet1!B55</f>
+        <f>Casos!B55</f>
         <v>130759</v>
       </c>
       <c r="C55">
@@ -22311,27 +23378,27 @@
         <v>2802.3789112730392</v>
       </c>
       <c r="D55">
-        <f>Sheet1!C55</f>
+        <f>Casos!C55</f>
         <v>17851</v>
       </c>
       <c r="F55">
-        <f>Sheet1!D54</f>
+        <f>Casos!D54</f>
         <v>124632</v>
       </c>
       <c r="H55">
-        <f>Sheet1!E54</f>
+        <f>Casos!E54</f>
         <v>85778</v>
       </c>
       <c r="J55">
-        <f>Sheet1!F54</f>
+        <f>Casos!F54</f>
         <v>68605</v>
       </c>
       <c r="L55">
-        <f>Sheet1!G54</f>
+        <f>Casos!G54</f>
         <v>41903</v>
       </c>
       <c r="N55">
-        <f>Sheet1!H55</f>
+        <f>Casos!H55</f>
         <v>304826</v>
       </c>
     </row>
@@ -22340,7 +23407,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <f>Sheet1!B56</f>
+        <f>Casos!B56</f>
         <v>135032</v>
       </c>
       <c r="C56">
@@ -22348,27 +23415,27 @@
         <v>2893.9562794684957</v>
       </c>
       <c r="D56">
-        <f>Sheet1!C56</f>
+        <f>Casos!C56</f>
         <v>17851</v>
       </c>
       <c r="F56">
-        <f>Sheet1!D56</f>
+        <f>Casos!D56</f>
         <v>128948</v>
       </c>
       <c r="H56">
-        <f>Sheet1!F56</f>
+        <f>Casos!F56</f>
         <v>70478</v>
       </c>
       <c r="J56" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="L56">
-        <f>Sheet1!G56</f>
+        <f>Casos!G56</f>
         <v>48451</v>
       </c>
       <c r="N56">
-        <f>Sheet1!H56</f>
+        <f>Casos!H56</f>
         <v>304826</v>
       </c>
     </row>
@@ -22377,7 +23444,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <f>Sheet1!B57</f>
+        <f>Casos!B57</f>
         <v>140510</v>
       </c>
       <c r="C57">
@@ -22385,27 +23452,27 @@
         <v>3011.3587655379342</v>
       </c>
       <c r="D57">
-        <f>Sheet1!C57</f>
+        <f>Casos!C57</f>
         <v>18803</v>
       </c>
       <c r="F57">
-        <f>Sheet1!D57</f>
+        <f>Casos!D57</f>
         <v>132547</v>
       </c>
       <c r="H57">
-        <f>Sheet1!E57</f>
+        <f>Casos!E57</f>
         <v>95391</v>
       </c>
       <c r="J57">
-        <f>Sheet1!F57</f>
+        <f>Casos!F57</f>
         <v>74390</v>
       </c>
       <c r="L57">
-        <f>Sheet1!G57</f>
+        <f>Casos!G57</f>
         <v>51608</v>
       </c>
       <c r="N57">
-        <f>Sheet1!H57</f>
+        <f>Casos!H57</f>
         <v>330891</v>
       </c>
     </row>
@@ -22414,7 +23481,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <f>Sheet1!B58</f>
+        <f>Casos!B58</f>
         <v>146690</v>
       </c>
       <c r="C58">
@@ -22422,27 +23489,27 @@
         <v>3143.8062580368628</v>
       </c>
       <c r="D58">
-        <f>Sheet1!C58</f>
+        <f>Casos!C58</f>
         <v>19580</v>
       </c>
       <c r="F58">
-        <f>Sheet1!D58</f>
+        <f>Casos!D58</f>
         <v>135586</v>
       </c>
       <c r="H58">
-        <f>Sheet1!E58</f>
+        <f>Casos!E58</f>
         <v>99225</v>
       </c>
       <c r="J58">
-        <f>Sheet1!F58</f>
+        <f>Casos!F58</f>
         <v>78167</v>
       </c>
       <c r="L58">
-        <f>Sheet1!G58</f>
+        <f>Casos!G58</f>
         <v>55242</v>
       </c>
       <c r="N58">
-        <f>Sheet1!H58</f>
+        <f>Casos!H58</f>
         <v>374329</v>
       </c>
     </row>
@@ -22451,7 +23518,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <f>Sheet1!B59</f>
+        <f>Casos!B59</f>
         <v>152446</v>
       </c>
       <c r="C59">
@@ -22459,27 +23526,27 @@
         <v>3267.166738105444</v>
       </c>
       <c r="D59" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="F59">
-        <f>Sheet1!D59</f>
+        <f>Casos!D59</f>
         <v>139422</v>
       </c>
       <c r="H59">
-        <f>Sheet1!E59</f>
+        <f>Casos!E59</f>
         <v>103228</v>
       </c>
       <c r="J59">
-        <f>Sheet1!F59</f>
+        <f>Casos!F59</f>
         <v>82048</v>
       </c>
       <c r="L59">
-        <f>Sheet1!G59</f>
+        <f>Casos!G59</f>
         <v>60733</v>
       </c>
       <c r="N59">
-        <f>Sheet1!C59</f>
+        <f>Casos!C59</f>
         <v>20549</v>
       </c>
     </row>
@@ -22488,7 +23555,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <f>Sheet1!B60</f>
+        <f>Casos!B60</f>
         <v>157022</v>
       </c>
       <c r="C60">
@@ -22496,27 +23563,27 @@
         <v>3365.237891127304</v>
       </c>
       <c r="D60">
-        <f>Sheet1!C60</f>
+        <f>Casos!C60</f>
         <v>21762</v>
       </c>
       <c r="F60">
-        <f>Sheet1!D60</f>
+        <f>Casos!D60</f>
         <v>143626</v>
       </c>
       <c r="H60">
-        <f>Sheet1!E60</f>
+        <f>Casos!E60</f>
         <v>108202</v>
       </c>
       <c r="J60">
-        <f>Sheet1!F60</f>
+        <f>Casos!F60</f>
         <v>86334</v>
       </c>
       <c r="L60">
-        <f>Sheet1!G60</f>
+        <f>Casos!G60</f>
         <v>65077</v>
       </c>
       <c r="N60">
-        <f>Sheet1!H60</f>
+        <f>Casos!H60</f>
         <v>427460</v>
       </c>
     </row>
@@ -22525,7 +23592,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <f>Sheet1!B61</f>
+        <f>Casos!B61</f>
         <v>0</v>
       </c>
       <c r="C61">
@@ -22533,27 +23600,27 @@
         <v>0</v>
       </c>
       <c r="D61">
-        <f>Sheet1!C61</f>
+        <f>Casos!C61</f>
         <v>0</v>
       </c>
       <c r="F61">
-        <f>Sheet1!D61</f>
+        <f>Casos!D61</f>
         <v>0</v>
       </c>
       <c r="H61">
-        <f>Sheet1!E61</f>
+        <f>Casos!E61</f>
         <v>0</v>
       </c>
       <c r="J61">
-        <f>Sheet1!F61</f>
+        <f>Casos!F61</f>
         <v>0</v>
       </c>
       <c r="L61">
-        <f>Sheet1!G61</f>
+        <f>Casos!G61</f>
         <v>0</v>
       </c>
       <c r="N61">
-        <f>Sheet1!H61</f>
+        <f>Casos!H61</f>
         <v>0</v>
       </c>
     </row>
@@ -22562,7 +23629,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <f>Sheet1!B62</f>
+        <f>Casos!B62</f>
         <v>0</v>
       </c>
       <c r="C62">
@@ -22570,27 +23637,27 @@
         <v>0</v>
       </c>
       <c r="D62">
-        <f>Sheet1!C62</f>
+        <f>Casos!C62</f>
         <v>0</v>
       </c>
       <c r="F62">
-        <f>Sheet1!D62</f>
+        <f>Casos!D62</f>
         <v>0</v>
       </c>
       <c r="H62">
-        <f>Sheet1!E62</f>
+        <f>Casos!E62</f>
         <v>0</v>
       </c>
       <c r="J62">
-        <f>Sheet1!F62</f>
+        <f>Casos!F62</f>
         <v>0</v>
       </c>
       <c r="L62">
-        <f>Sheet1!G62</f>
+        <f>Casos!G62</f>
         <v>0</v>
       </c>
       <c r="N62">
-        <f>Sheet1!H62</f>
+        <f>Casos!H62</f>
         <v>0</v>
       </c>
     </row>
@@ -22599,7 +23666,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <f>Sheet1!B63</f>
+        <f>Casos!B63</f>
         <v>0</v>
       </c>
       <c r="C63">
@@ -22607,27 +23674,27 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <f>Sheet1!C63</f>
+        <f>Casos!C63</f>
         <v>0</v>
       </c>
       <c r="F63">
-        <f>Sheet1!D63</f>
+        <f>Casos!D63</f>
         <v>0</v>
       </c>
       <c r="H63">
-        <f>Sheet1!E63</f>
+        <f>Casos!E63</f>
         <v>0</v>
       </c>
       <c r="J63">
-        <f>Sheet1!F63</f>
+        <f>Casos!F63</f>
         <v>0</v>
       </c>
       <c r="L63">
-        <f>Sheet1!G63</f>
+        <f>Casos!G63</f>
         <v>0</v>
       </c>
       <c r="N63">
-        <f>Sheet1!H63</f>
+        <f>Casos!H63</f>
         <v>0</v>
       </c>
     </row>
@@ -22636,7 +23703,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <f>Sheet1!B64</f>
+        <f>Casos!B64</f>
         <v>0</v>
       </c>
       <c r="C64">
@@ -22644,27 +23711,27 @@
         <v>0</v>
       </c>
       <c r="D64">
-        <f>Sheet1!C64</f>
+        <f>Casos!C64</f>
         <v>0</v>
       </c>
       <c r="F64">
-        <f>Sheet1!D64</f>
+        <f>Casos!D64</f>
         <v>0</v>
       </c>
       <c r="H64">
-        <f>Sheet1!E64</f>
+        <f>Casos!E64</f>
         <v>0</v>
       </c>
       <c r="J64">
-        <f>Sheet1!F64</f>
+        <f>Casos!F64</f>
         <v>0</v>
       </c>
       <c r="L64">
-        <f>Sheet1!G64</f>
+        <f>Casos!G64</f>
         <v>0</v>
       </c>
       <c r="N64">
-        <f>Sheet1!H64</f>
+        <f>Casos!H64</f>
         <v>0</v>
       </c>
     </row>
@@ -22673,7 +23740,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <f>Sheet1!B65</f>
+        <f>Casos!B65</f>
         <v>0</v>
       </c>
       <c r="C65">
@@ -22681,27 +23748,27 @@
         <v>0</v>
       </c>
       <c r="D65">
-        <f>Sheet1!C65</f>
+        <f>Casos!C65</f>
         <v>0</v>
       </c>
       <c r="F65">
-        <f>Sheet1!D65</f>
+        <f>Casos!D65</f>
         <v>0</v>
       </c>
       <c r="H65">
-        <f>Sheet1!E65</f>
+        <f>Casos!E65</f>
         <v>0</v>
       </c>
       <c r="J65">
-        <f>Sheet1!F65</f>
+        <f>Casos!F65</f>
         <v>0</v>
       </c>
       <c r="L65">
-        <f>Sheet1!G65</f>
+        <f>Casos!G65</f>
         <v>0</v>
       </c>
       <c r="N65">
-        <f>Sheet1!H65</f>
+        <f>Casos!H65</f>
         <v>0</v>
       </c>
     </row>
@@ -22710,7 +23777,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <f>Sheet1!B66</f>
+        <f>Casos!B66</f>
         <v>0</v>
       </c>
       <c r="C66">
@@ -22718,27 +23785,27 @@
         <v>0</v>
       </c>
       <c r="D66">
-        <f>Sheet1!C66</f>
+        <f>Casos!C66</f>
         <v>0</v>
       </c>
       <c r="F66">
-        <f>Sheet1!D66</f>
+        <f>Casos!D66</f>
         <v>0</v>
       </c>
       <c r="H66">
-        <f>Sheet1!E66</f>
+        <f>Casos!E66</f>
         <v>0</v>
       </c>
       <c r="J66">
-        <f>Sheet1!F66</f>
+        <f>Casos!F66</f>
         <v>0</v>
       </c>
       <c r="L66">
-        <f>Sheet1!G66</f>
+        <f>Casos!G66</f>
         <v>0</v>
       </c>
       <c r="N66">
-        <f>Sheet1!H66</f>
+        <f>Casos!H66</f>
         <v>0</v>
       </c>
     </row>
@@ -22747,7 +23814,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <f>Sheet1!B67</f>
+        <f>Casos!B67</f>
         <v>0</v>
       </c>
       <c r="C67">
@@ -22755,27 +23822,27 @@
         <v>0</v>
       </c>
       <c r="D67">
-        <f>Sheet1!C67</f>
+        <f>Casos!C67</f>
         <v>0</v>
       </c>
       <c r="F67">
-        <f>Sheet1!D67</f>
+        <f>Casos!D67</f>
         <v>0</v>
       </c>
       <c r="H67">
-        <f>Sheet1!E67</f>
+        <f>Casos!E67</f>
         <v>0</v>
       </c>
       <c r="J67">
-        <f>Sheet1!F67</f>
+        <f>Casos!F67</f>
         <v>0</v>
       </c>
       <c r="L67">
-        <f>Sheet1!G67</f>
+        <f>Casos!G67</f>
         <v>0</v>
       </c>
       <c r="N67">
-        <f>Sheet1!H67</f>
+        <f>Casos!H67</f>
         <v>0</v>
       </c>
     </row>
@@ -22784,7 +23851,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <f>Sheet1!B68</f>
+        <f>Casos!B68</f>
         <v>0</v>
       </c>
       <c r="C68">
@@ -22792,27 +23859,27 @@
         <v>0</v>
       </c>
       <c r="D68">
-        <f>Sheet1!C68</f>
+        <f>Casos!C68</f>
         <v>0</v>
       </c>
       <c r="F68">
-        <f>Sheet1!D68</f>
+        <f>Casos!D68</f>
         <v>0</v>
       </c>
       <c r="H68">
-        <f>Sheet1!E68</f>
+        <f>Casos!E68</f>
         <v>0</v>
       </c>
       <c r="J68">
-        <f>Sheet1!F68</f>
+        <f>Casos!F68</f>
         <v>0</v>
       </c>
       <c r="L68">
-        <f>Sheet1!G68</f>
+        <f>Casos!G68</f>
         <v>0</v>
       </c>
       <c r="N68">
-        <f>Sheet1!H68</f>
+        <f>Casos!H68</f>
         <v>0</v>
       </c>
     </row>
@@ -22821,7 +23888,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <f>Sheet1!B69</f>
+        <f>Casos!B69</f>
         <v>0</v>
       </c>
       <c r="C69">
@@ -22829,27 +23896,27 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <f>Sheet1!C69</f>
+        <f>Casos!C69</f>
         <v>0</v>
       </c>
       <c r="F69">
-        <f>Sheet1!D69</f>
+        <f>Casos!D69</f>
         <v>0</v>
       </c>
       <c r="H69">
-        <f>Sheet1!E69</f>
+        <f>Casos!E69</f>
         <v>0</v>
       </c>
       <c r="J69">
-        <f>Sheet1!F69</f>
+        <f>Casos!F69</f>
         <v>0</v>
       </c>
       <c r="L69">
-        <f>Sheet1!G69</f>
+        <f>Casos!G69</f>
         <v>0</v>
       </c>
       <c r="N69">
-        <f>Sheet1!H69</f>
+        <f>Casos!H69</f>
         <v>0</v>
       </c>
     </row>
@@ -22858,7 +23925,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <f>Sheet1!B70</f>
+        <f>Casos!B70</f>
         <v>0</v>
       </c>
       <c r="C70">
@@ -22866,27 +23933,27 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <f>Sheet1!C70</f>
+        <f>Casos!C70</f>
         <v>0</v>
       </c>
       <c r="F70">
-        <f>Sheet1!D70</f>
+        <f>Casos!D70</f>
         <v>0</v>
       </c>
       <c r="H70">
-        <f>Sheet1!E70</f>
+        <f>Casos!E70</f>
         <v>0</v>
       </c>
       <c r="J70">
-        <f>Sheet1!F70</f>
+        <f>Casos!F70</f>
         <v>0</v>
       </c>
       <c r="L70">
-        <f>Sheet1!G70</f>
+        <f>Casos!G70</f>
         <v>0</v>
       </c>
       <c r="N70">
-        <f>Sheet1!H70</f>
+        <f>Casos!H70</f>
         <v>0</v>
       </c>
     </row>
@@ -22896,7 +23963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AJ70"/>
   <sheetViews>
@@ -25144,7 +26211,7 @@
         <v>1372.8889841405917</v>
       </c>
       <c r="D46">
-        <f>Sheet1!C46</f>
+        <f>Casos!C46</f>
         <v>8603</v>
       </c>
       <c r="E46">
@@ -25152,7 +26219,7 @@
         <v>500.75669383003492</v>
       </c>
       <c r="F46">
-        <f>Sheet1!D46</f>
+        <f>Casos!D46</f>
         <v>86498</v>
       </c>
       <c r="G46">
@@ -25160,7 +26227,7 @@
         <v>1430.1917989417991</v>
       </c>
       <c r="H46">
-        <f>Sheet1!E46</f>
+        <f>Casos!E46</f>
         <v>48582</v>
       </c>
       <c r="I46">
@@ -25168,7 +26235,7 @@
         <v>586.8100012078753</v>
       </c>
       <c r="J46">
-        <f>Sheet1!F46</f>
+        <f>Casos!F46</f>
         <v>32964</v>
       </c>
       <c r="K46">
@@ -25176,7 +26243,7 @@
         <v>492.07344379758177</v>
       </c>
       <c r="L46">
-        <f>Sheet1!G46</f>
+        <f>Casos!G46</f>
         <v>14543</v>
       </c>
       <c r="M46">
@@ -25199,7 +26266,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <f>Sheet1!B47</f>
+        <f>Casos!B47</f>
         <v>72248</v>
       </c>
       <c r="C47">
@@ -25207,7 +26274,7 @@
         <v>1548.3926275182171</v>
       </c>
       <c r="D47">
-        <f>Sheet1!C47</f>
+        <f>Casos!C47</f>
         <v>9762</v>
       </c>
       <c r="E47">
@@ -25215,7 +26282,7 @@
         <v>568.21885913853316</v>
       </c>
       <c r="F47">
-        <f>Sheet1!D47</f>
+        <f>Casos!D47</f>
         <v>92472</v>
       </c>
       <c r="G47">
@@ -25223,7 +26290,7 @@
         <v>1528.968253968254</v>
       </c>
       <c r="H47">
-        <f>Sheet1!E47</f>
+        <f>Casos!E47</f>
         <v>52547</v>
       </c>
       <c r="I47">
@@ -25231,7 +26298,7 @@
         <v>634.70225872689934</v>
       </c>
       <c r="J47">
-        <f>Sheet1!F47</f>
+        <f>Casos!F47</f>
         <v>37575</v>
       </c>
       <c r="K47">
@@ -25239,7 +26306,7 @@
         <v>560.90461262875056</v>
       </c>
       <c r="L47">
-        <f>Sheet1!G47</f>
+        <f>Casos!G47</f>
         <v>17089</v>
       </c>
       <c r="M47">
@@ -25262,7 +26329,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <f>Sheet1!B48</f>
+        <f>Casos!B48</f>
         <v>78797</v>
       </c>
       <c r="C48">
@@ -25270,7 +26337,7 @@
         <v>1688.7483926275183</v>
       </c>
       <c r="D48">
-        <f>Sheet1!C48</f>
+        <f>Casos!C48</f>
         <v>10866</v>
       </c>
       <c r="E48">
@@ -25278,7 +26345,7 @@
         <v>632.47962747380677</v>
       </c>
       <c r="F48">
-        <f>Sheet1!D48</f>
+        <f>Casos!D48</f>
         <v>97689</v>
       </c>
       <c r="G48">
@@ -25286,7 +26353,7 @@
         <v>1615.2281746031747</v>
       </c>
       <c r="H48">
-        <f>Sheet1!E48</f>
+        <f>Casos!E48</f>
         <v>57298</v>
       </c>
       <c r="I48">
@@ -25294,7 +26361,7 @@
         <v>692.08841647541965</v>
       </c>
       <c r="J48">
-        <f>Sheet1!F48</f>
+        <f>Casos!F48</f>
         <v>40174</v>
       </c>
       <c r="K48">
@@ -25302,7 +26369,7 @@
         <v>599.70144797731007</v>
       </c>
       <c r="L48">
-        <f>Sheet1!G48</f>
+        <f>Casos!G48</f>
         <v>19522</v>
       </c>
       <c r="M48">
@@ -25310,7 +26377,7 @@
         <v>293.82901866345577</v>
       </c>
       <c r="N48">
-        <f>Sheet1!H49</f>
+        <f>Casos!H49</f>
         <v>143025</v>
       </c>
       <c r="O48">
@@ -25326,7 +26393,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <f>Sheet1!B49</f>
+        <f>Casos!B49</f>
         <v>85195</v>
       </c>
       <c r="C49">
@@ -25334,7 +26401,7 @@
         <v>1825.867981140163</v>
       </c>
       <c r="D49">
-        <f>Sheet1!C49</f>
+        <f>Casos!C49</f>
         <v>11750</v>
       </c>
       <c r="E49">
@@ -25342,7 +26409,7 @@
         <v>683.93480791618163</v>
       </c>
       <c r="F49">
-        <f>Sheet1!D49</f>
+        <f>Casos!D49</f>
         <v>101739</v>
       </c>
       <c r="G49">
@@ -25350,7 +26417,7 @@
         <v>1682.1924603174605</v>
       </c>
       <c r="H49">
-        <f>Sheet1!E49</f>
+        <f>Casos!E49</f>
         <v>61913</v>
       </c>
       <c r="I49">
@@ -25358,7 +26425,7 @@
         <v>747.83186375166076</v>
       </c>
       <c r="J49">
-        <f>Sheet1!F49</f>
+        <f>Casos!F49</f>
         <v>44550</v>
       </c>
       <c r="K49">
@@ -25366,7 +26433,7 @@
         <v>665.02463054187194</v>
       </c>
       <c r="L49">
-        <f>Sheet1!G49</f>
+        <f>Casos!G49</f>
         <v>22141</v>
       </c>
       <c r="M49">
@@ -25374,7 +26441,7 @@
         <v>333.2480433473811</v>
       </c>
       <c r="N49">
-        <f>Sheet1!H50</f>
+        <f>Casos!H50</f>
         <v>163539</v>
       </c>
       <c r="O49">
@@ -25390,7 +26457,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <f>Sheet1!B50</f>
+        <f>Casos!B50</f>
         <v>94417</v>
       </c>
       <c r="C50">
@@ -25398,7 +26465,7 @@
         <v>2023.5105015002146</v>
       </c>
       <c r="D50">
-        <f>Sheet1!C50</f>
+        <f>Casos!C50</f>
         <v>12595</v>
       </c>
       <c r="E50">
@@ -25406,7 +26473,7 @@
         <v>733.11990686845172</v>
       </c>
       <c r="F50">
-        <f>Sheet1!D50</f>
+        <f>Casos!D50</f>
         <v>105792</v>
       </c>
       <c r="G50">
@@ -25414,7 +26481,7 @@
         <v>1749.2063492063494</v>
       </c>
       <c r="H50">
-        <f>Sheet1!E50</f>
+        <f>Casos!E50</f>
         <v>67366</v>
       </c>
       <c r="I50">
@@ -25422,7 +26489,7 @@
         <v>813.6973064379755</v>
       </c>
       <c r="J50">
-        <f>Sheet1!F50</f>
+        <f>Casos!F50</f>
         <v>52128</v>
       </c>
       <c r="K50">
@@ -25430,7 +26497,7 @@
         <v>778.14599193909544</v>
       </c>
       <c r="L50">
-        <f>Sheet1!G50</f>
+        <f>Casos!G50</f>
         <v>25150</v>
       </c>
       <c r="M50">
@@ -25438,7 +26505,7 @@
         <v>378.53702588801929</v>
       </c>
       <c r="N50">
-        <f>Sheet1!H51</f>
+        <f>Casos!H51</f>
         <v>186101</v>
       </c>
       <c r="O50">
@@ -25454,7 +26521,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <f>Sheet1!B51</f>
+        <f>Casos!B51</f>
         <v>102136</v>
       </c>
       <c r="C51">
@@ -25462,7 +26529,7 @@
         <v>2188.9412773253325</v>
       </c>
       <c r="D51">
-        <f>Sheet1!C51</f>
+        <f>Casos!C51</f>
         <v>13614</v>
       </c>
       <c r="E51">
@@ -25470,7 +26537,7 @@
         <v>792.43306169965081</v>
       </c>
       <c r="F51">
-        <f>Sheet1!D51</f>
+        <f>Casos!D51</f>
         <v>110574</v>
       </c>
       <c r="G51">
@@ -25478,7 +26545,7 @@
         <v>1828.2738095238096</v>
       </c>
       <c r="H51">
-        <f>Sheet1!E51</f>
+        <f>Casos!E51</f>
         <v>73522</v>
       </c>
       <c r="I51">
@@ -25486,7 +26553,7 @@
         <v>888.05411281555735</v>
       </c>
       <c r="J51">
-        <f>Sheet1!F51</f>
+        <f>Casos!F51</f>
         <v>56989</v>
       </c>
       <c r="K51">
@@ -25494,7 +26561,7 @@
         <v>850.70906105388872</v>
       </c>
       <c r="L51">
-        <f>Sheet1!G51</f>
+        <f>Casos!G51</f>
         <v>29474</v>
       </c>
       <c r="M51">
@@ -25502,7 +26569,7 @@
         <v>443.61830222757379</v>
       </c>
       <c r="N51" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="O51" t="e">
@@ -25518,7 +26585,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <f>Sheet1!B52</f>
+        <f>Casos!B52</f>
         <v>110238</v>
       </c>
       <c r="C52">
@@ -25526,7 +26593,7 @@
         <v>2362.5803686240893</v>
       </c>
       <c r="D52">
-        <f>Sheet1!C52</f>
+        <f>Casos!C52</f>
         <v>13614</v>
       </c>
       <c r="E52">
@@ -25534,7 +26601,7 @@
         <v>792.43306169965081</v>
       </c>
       <c r="F52">
-        <f>Sheet1!D52</f>
+        <f>Casos!D52</f>
         <v>115242</v>
       </c>
       <c r="G52">
@@ -25542,7 +26609,7 @@
         <v>1905.4563492063494</v>
       </c>
       <c r="H52">
-        <f>Sheet1!E52</f>
+        <f>Casos!E52</f>
         <v>73522</v>
       </c>
       <c r="I52">
@@ -25550,7 +26617,7 @@
         <v>888.05411281555735</v>
       </c>
       <c r="J52">
-        <f>Sheet1!F52</f>
+        <f>Casos!F52</f>
         <v>59105</v>
       </c>
       <c r="K52">
@@ -25558,7 +26625,7 @@
         <v>882.29586505448583</v>
       </c>
       <c r="L52">
-        <f>Sheet1!G52</f>
+        <f>Casos!G52</f>
         <v>33718</v>
       </c>
       <c r="M52">
@@ -25566,7 +26633,7 @@
         <v>507.49548464780253</v>
       </c>
       <c r="N52">
-        <f>Sheet1!H52</f>
+        <f>Casos!H52</f>
         <v>213144</v>
       </c>
       <c r="O52">
@@ -25581,7 +26648,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <f>Sheet1!B53</f>
+        <f>Casos!B53</f>
         <v>117710</v>
       </c>
       <c r="C53">
@@ -25589,27 +26656,27 @@
         <v>2522.717531075868</v>
       </c>
       <c r="D53">
-        <f>Sheet1!C53</f>
+        <f>Casos!C53</f>
         <v>15723</v>
       </c>
       <c r="F53">
-        <f>Sheet1!D53</f>
+        <f>Casos!D53</f>
         <v>119827</v>
       </c>
       <c r="H53" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="J53">
-        <f>Sheet1!E53</f>
+        <f>Casos!E53</f>
         <v>79696</v>
       </c>
       <c r="L53">
-        <f>Sheet1!G53</f>
+        <f>Casos!G53</f>
         <v>38168</v>
       </c>
       <c r="N53">
-        <f>Sheet1!H53</f>
+        <f>Casos!H53</f>
         <v>239279</v>
       </c>
     </row>
@@ -25618,31 +26685,31 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <f>Sheet1!B54</f>
+        <f>Casos!B54</f>
         <v>124736</v>
       </c>
       <c r="D54">
-        <f>Sheet1!C54</f>
+        <f>Casos!C54</f>
         <v>16627</v>
       </c>
       <c r="F54" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="H54" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="J54" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="L54" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="N54">
-        <f>Sheet1!H54</f>
+        <f>Casos!H54</f>
         <v>277205</v>
       </c>
     </row>
@@ -25651,31 +26718,31 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <f>Sheet1!B55</f>
+        <f>Casos!B55</f>
         <v>130759</v>
       </c>
       <c r="D55">
-        <f>Sheet1!C55</f>
+        <f>Casos!C55</f>
         <v>17851</v>
       </c>
       <c r="F55">
-        <f>Sheet1!D54</f>
+        <f>Casos!D54</f>
         <v>124632</v>
       </c>
       <c r="H55">
-        <f>Sheet1!E54</f>
+        <f>Casos!E54</f>
         <v>85778</v>
       </c>
       <c r="J55">
-        <f>Sheet1!F54</f>
+        <f>Casos!F54</f>
         <v>68605</v>
       </c>
       <c r="L55">
-        <f>Sheet1!G54</f>
+        <f>Casos!G54</f>
         <v>41903</v>
       </c>
       <c r="N55">
-        <f>Sheet1!H55</f>
+        <f>Casos!H55</f>
         <v>304826</v>
       </c>
     </row>
@@ -25684,31 +26751,31 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <f>Sheet1!B56</f>
+        <f>Casos!B56</f>
         <v>135032</v>
       </c>
       <c r="D56">
-        <f>Sheet1!C56</f>
+        <f>Casos!C56</f>
         <v>17851</v>
       </c>
       <c r="F56">
-        <f>Sheet1!D56</f>
+        <f>Casos!D56</f>
         <v>128948</v>
       </c>
       <c r="H56">
-        <f>Sheet1!F56</f>
+        <f>Casos!F56</f>
         <v>70478</v>
       </c>
       <c r="J56" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="L56">
-        <f>Sheet1!G56</f>
+        <f>Casos!G56</f>
         <v>48451</v>
       </c>
       <c r="N56">
-        <f>Sheet1!H56</f>
+        <f>Casos!H56</f>
         <v>304826</v>
       </c>
     </row>
@@ -25717,31 +26784,31 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <f>Sheet1!B57</f>
+        <f>Casos!B57</f>
         <v>140510</v>
       </c>
       <c r="D57">
-        <f>Sheet1!C57</f>
+        <f>Casos!C57</f>
         <v>18803</v>
       </c>
       <c r="F57">
-        <f>Sheet1!D57</f>
+        <f>Casos!D57</f>
         <v>132547</v>
       </c>
       <c r="H57">
-        <f>Sheet1!E57</f>
+        <f>Casos!E57</f>
         <v>95391</v>
       </c>
       <c r="J57">
-        <f>Sheet1!F57</f>
+        <f>Casos!F57</f>
         <v>74390</v>
       </c>
       <c r="L57">
-        <f>Sheet1!G57</f>
+        <f>Casos!G57</f>
         <v>51608</v>
       </c>
       <c r="N57">
-        <f>Sheet1!H57</f>
+        <f>Casos!H57</f>
         <v>330891</v>
       </c>
     </row>
@@ -25750,31 +26817,31 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <f>Sheet1!B58</f>
+        <f>Casos!B58</f>
         <v>146690</v>
       </c>
       <c r="D58">
-        <f>Sheet1!C58</f>
+        <f>Casos!C58</f>
         <v>19580</v>
       </c>
       <c r="F58">
-        <f>Sheet1!D58</f>
+        <f>Casos!D58</f>
         <v>135586</v>
       </c>
       <c r="H58">
-        <f>Sheet1!E58</f>
+        <f>Casos!E58</f>
         <v>99225</v>
       </c>
       <c r="J58">
-        <f>Sheet1!F58</f>
+        <f>Casos!F58</f>
         <v>78167</v>
       </c>
       <c r="L58">
-        <f>Sheet1!G58</f>
+        <f>Casos!G58</f>
         <v>55242</v>
       </c>
       <c r="N58">
-        <f>Sheet1!H58</f>
+        <f>Casos!H58</f>
         <v>374329</v>
       </c>
     </row>
@@ -25783,31 +26850,31 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <f>Sheet1!B59</f>
+        <f>Casos!B59</f>
         <v>152446</v>
       </c>
       <c r="D59" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="F59">
-        <f>Sheet1!D59</f>
+        <f>Casos!D59</f>
         <v>139422</v>
       </c>
       <c r="H59">
-        <f>Sheet1!E59</f>
+        <f>Casos!E59</f>
         <v>103228</v>
       </c>
       <c r="J59">
-        <f>Sheet1!F59</f>
+        <f>Casos!F59</f>
         <v>82048</v>
       </c>
       <c r="L59">
-        <f>Sheet1!G59</f>
+        <f>Casos!G59</f>
         <v>60733</v>
       </c>
       <c r="N59">
-        <f>Sheet1!C59</f>
+        <f>Casos!C59</f>
         <v>20549</v>
       </c>
     </row>
@@ -25816,31 +26883,31 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <f>Sheet1!B60</f>
+        <f>Casos!B60</f>
         <v>157022</v>
       </c>
       <c r="D60">
-        <f>Sheet1!C60</f>
+        <f>Casos!C60</f>
         <v>21762</v>
       </c>
       <c r="F60">
-        <f>Sheet1!D60</f>
+        <f>Casos!D60</f>
         <v>143626</v>
       </c>
       <c r="H60">
-        <f>Sheet1!E60</f>
+        <f>Casos!E60</f>
         <v>108202</v>
       </c>
       <c r="J60">
-        <f>Sheet1!F60</f>
+        <f>Casos!F60</f>
         <v>86334</v>
       </c>
       <c r="L60">
-        <f>Sheet1!G60</f>
+        <f>Casos!G60</f>
         <v>65077</v>
       </c>
       <c r="N60">
-        <f>Sheet1!H60</f>
+        <f>Casos!H60</f>
         <v>427460</v>
       </c>
     </row>
@@ -25849,31 +26916,31 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <f>Sheet1!B61</f>
+        <f>Casos!B61</f>
         <v>0</v>
       </c>
       <c r="D61">
-        <f>Sheet1!C61</f>
+        <f>Casos!C61</f>
         <v>0</v>
       </c>
       <c r="F61">
-        <f>Sheet1!D61</f>
+        <f>Casos!D61</f>
         <v>0</v>
       </c>
       <c r="H61">
-        <f>Sheet1!E61</f>
+        <f>Casos!E61</f>
         <v>0</v>
       </c>
       <c r="J61">
-        <f>Sheet1!F61</f>
+        <f>Casos!F61</f>
         <v>0</v>
       </c>
       <c r="L61">
-        <f>Sheet1!G61</f>
+        <f>Casos!G61</f>
         <v>0</v>
       </c>
       <c r="N61">
-        <f>Sheet1!H61</f>
+        <f>Casos!H61</f>
         <v>0</v>
       </c>
     </row>
@@ -25882,31 +26949,31 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <f>Sheet1!B62</f>
+        <f>Casos!B62</f>
         <v>0</v>
       </c>
       <c r="D62">
-        <f>Sheet1!C62</f>
+        <f>Casos!C62</f>
         <v>0</v>
       </c>
       <c r="F62">
-        <f>Sheet1!D62</f>
+        <f>Casos!D62</f>
         <v>0</v>
       </c>
       <c r="H62">
-        <f>Sheet1!E62</f>
+        <f>Casos!E62</f>
         <v>0</v>
       </c>
       <c r="J62">
-        <f>Sheet1!F62</f>
+        <f>Casos!F62</f>
         <v>0</v>
       </c>
       <c r="L62">
-        <f>Sheet1!G62</f>
+        <f>Casos!G62</f>
         <v>0</v>
       </c>
       <c r="N62">
-        <f>Sheet1!H62</f>
+        <f>Casos!H62</f>
         <v>0</v>
       </c>
     </row>
@@ -25915,31 +26982,31 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <f>Sheet1!B63</f>
+        <f>Casos!B63</f>
         <v>0</v>
       </c>
       <c r="D63">
-        <f>Sheet1!C63</f>
+        <f>Casos!C63</f>
         <v>0</v>
       </c>
       <c r="F63">
-        <f>Sheet1!D63</f>
+        <f>Casos!D63</f>
         <v>0</v>
       </c>
       <c r="H63">
-        <f>Sheet1!E63</f>
+        <f>Casos!E63</f>
         <v>0</v>
       </c>
       <c r="J63">
-        <f>Sheet1!F63</f>
+        <f>Casos!F63</f>
         <v>0</v>
       </c>
       <c r="L63">
-        <f>Sheet1!G63</f>
+        <f>Casos!G63</f>
         <v>0</v>
       </c>
       <c r="N63">
-        <f>Sheet1!H63</f>
+        <f>Casos!H63</f>
         <v>0</v>
       </c>
     </row>
@@ -25948,31 +27015,31 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <f>Sheet1!B64</f>
+        <f>Casos!B64</f>
         <v>0</v>
       </c>
       <c r="D64">
-        <f>Sheet1!C64</f>
+        <f>Casos!C64</f>
         <v>0</v>
       </c>
       <c r="F64">
-        <f>Sheet1!D64</f>
+        <f>Casos!D64</f>
         <v>0</v>
       </c>
       <c r="H64">
-        <f>Sheet1!E64</f>
+        <f>Casos!E64</f>
         <v>0</v>
       </c>
       <c r="J64">
-        <f>Sheet1!F64</f>
+        <f>Casos!F64</f>
         <v>0</v>
       </c>
       <c r="L64">
-        <f>Sheet1!G64</f>
+        <f>Casos!G64</f>
         <v>0</v>
       </c>
       <c r="N64">
-        <f>Sheet1!H64</f>
+        <f>Casos!H64</f>
         <v>0</v>
       </c>
     </row>
@@ -25981,31 +27048,31 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <f>Sheet1!B65</f>
+        <f>Casos!B65</f>
         <v>0</v>
       </c>
       <c r="D65">
-        <f>Sheet1!C65</f>
+        <f>Casos!C65</f>
         <v>0</v>
       </c>
       <c r="F65">
-        <f>Sheet1!D65</f>
+        <f>Casos!D65</f>
         <v>0</v>
       </c>
       <c r="H65">
-        <f>Sheet1!E65</f>
+        <f>Casos!E65</f>
         <v>0</v>
       </c>
       <c r="J65">
-        <f>Sheet1!F65</f>
+        <f>Casos!F65</f>
         <v>0</v>
       </c>
       <c r="L65">
-        <f>Sheet1!G65</f>
+        <f>Casos!G65</f>
         <v>0</v>
       </c>
       <c r="N65">
-        <f>Sheet1!H65</f>
+        <f>Casos!H65</f>
         <v>0</v>
       </c>
     </row>
@@ -26014,31 +27081,31 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <f>Sheet1!B66</f>
+        <f>Casos!B66</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f>Sheet1!C66</f>
+        <f>Casos!C66</f>
         <v>0</v>
       </c>
       <c r="F66">
-        <f>Sheet1!D66</f>
+        <f>Casos!D66</f>
         <v>0</v>
       </c>
       <c r="H66">
-        <f>Sheet1!E66</f>
+        <f>Casos!E66</f>
         <v>0</v>
       </c>
       <c r="J66">
-        <f>Sheet1!F66</f>
+        <f>Casos!F66</f>
         <v>0</v>
       </c>
       <c r="L66">
-        <f>Sheet1!G66</f>
+        <f>Casos!G66</f>
         <v>0</v>
       </c>
       <c r="N66">
-        <f>Sheet1!H66</f>
+        <f>Casos!H66</f>
         <v>0</v>
       </c>
     </row>
@@ -26047,31 +27114,31 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <f>Sheet1!B67</f>
+        <f>Casos!B67</f>
         <v>0</v>
       </c>
       <c r="D67">
-        <f>Sheet1!C67</f>
+        <f>Casos!C67</f>
         <v>0</v>
       </c>
       <c r="F67">
-        <f>Sheet1!D67</f>
+        <f>Casos!D67</f>
         <v>0</v>
       </c>
       <c r="H67">
-        <f>Sheet1!E67</f>
+        <f>Casos!E67</f>
         <v>0</v>
       </c>
       <c r="J67">
-        <f>Sheet1!F67</f>
+        <f>Casos!F67</f>
         <v>0</v>
       </c>
       <c r="L67">
-        <f>Sheet1!G67</f>
+        <f>Casos!G67</f>
         <v>0</v>
       </c>
       <c r="N67">
-        <f>Sheet1!H67</f>
+        <f>Casos!H67</f>
         <v>0</v>
       </c>
     </row>
@@ -26080,31 +27147,31 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <f>Sheet1!B68</f>
+        <f>Casos!B68</f>
         <v>0</v>
       </c>
       <c r="D68">
-        <f>Sheet1!C68</f>
+        <f>Casos!C68</f>
         <v>0</v>
       </c>
       <c r="F68">
-        <f>Sheet1!D68</f>
+        <f>Casos!D68</f>
         <v>0</v>
       </c>
       <c r="H68">
-        <f>Sheet1!E68</f>
+        <f>Casos!E68</f>
         <v>0</v>
       </c>
       <c r="J68">
-        <f>Sheet1!F68</f>
+        <f>Casos!F68</f>
         <v>0</v>
       </c>
       <c r="L68">
-        <f>Sheet1!G68</f>
+        <f>Casos!G68</f>
         <v>0</v>
       </c>
       <c r="N68">
-        <f>Sheet1!H68</f>
+        <f>Casos!H68</f>
         <v>0</v>
       </c>
     </row>
@@ -26113,31 +27180,31 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <f>Sheet1!B69</f>
+        <f>Casos!B69</f>
         <v>0</v>
       </c>
       <c r="D69">
-        <f>Sheet1!C69</f>
+        <f>Casos!C69</f>
         <v>0</v>
       </c>
       <c r="F69">
-        <f>Sheet1!D69</f>
+        <f>Casos!D69</f>
         <v>0</v>
       </c>
       <c r="H69">
-        <f>Sheet1!E69</f>
+        <f>Casos!E69</f>
         <v>0</v>
       </c>
       <c r="J69">
-        <f>Sheet1!F69</f>
+        <f>Casos!F69</f>
         <v>0</v>
       </c>
       <c r="L69">
-        <f>Sheet1!G69</f>
+        <f>Casos!G69</f>
         <v>0</v>
       </c>
       <c r="N69">
-        <f>Sheet1!H69</f>
+        <f>Casos!H69</f>
         <v>0</v>
       </c>
     </row>
@@ -26146,31 +27213,31 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <f>Sheet1!B70</f>
+        <f>Casos!B70</f>
         <v>0</v>
       </c>
       <c r="D70">
-        <f>Sheet1!C70</f>
+        <f>Casos!C70</f>
         <v>0</v>
       </c>
       <c r="F70">
-        <f>Sheet1!D70</f>
+        <f>Casos!D70</f>
         <v>0</v>
       </c>
       <c r="H70">
-        <f>Sheet1!E70</f>
+        <f>Casos!E70</f>
         <v>0</v>
       </c>
       <c r="J70">
-        <f>Sheet1!F70</f>
+        <f>Casos!F70</f>
         <v>0</v>
       </c>
       <c r="L70">
-        <f>Sheet1!G70</f>
+        <f>Casos!G70</f>
         <v>0</v>
       </c>
       <c r="N70">
-        <f>Sheet1!H70</f>
+        <f>Casos!H70</f>
         <v>0</v>
       </c>
     </row>
@@ -26180,7 +27247,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AJ70"/>
   <sheetViews>
@@ -28428,7 +29495,7 @@
         <v>1372.8889841405917</v>
       </c>
       <c r="D46">
-        <f>Sheet1!C46</f>
+        <f>Casos!C46</f>
         <v>8603</v>
       </c>
       <c r="E46">
@@ -28436,7 +29503,7 @@
         <v>500.75669383003492</v>
       </c>
       <c r="F46">
-        <f>Sheet1!D46</f>
+        <f>Casos!D46</f>
         <v>86498</v>
       </c>
       <c r="G46">
@@ -28444,7 +29511,7 @@
         <v>1430.1917989417991</v>
       </c>
       <c r="H46">
-        <f>Sheet1!E46</f>
+        <f>Casos!E46</f>
         <v>48582</v>
       </c>
       <c r="I46">
@@ -28452,7 +29519,7 @@
         <v>586.8100012078753</v>
       </c>
       <c r="J46">
-        <f>Sheet1!F46</f>
+        <f>Casos!F46</f>
         <v>32964</v>
       </c>
       <c r="K46">
@@ -28460,7 +29527,7 @@
         <v>492.07344379758177</v>
       </c>
       <c r="L46">
-        <f>Sheet1!G46</f>
+        <f>Casos!G46</f>
         <v>14543</v>
       </c>
       <c r="M46">
@@ -28483,7 +29550,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <f>Sheet1!B47</f>
+        <f>Casos!B47</f>
         <v>72248</v>
       </c>
       <c r="C47">
@@ -28491,7 +29558,7 @@
         <v>1548.3926275182171</v>
       </c>
       <c r="D47">
-        <f>Sheet1!C47</f>
+        <f>Casos!C47</f>
         <v>9762</v>
       </c>
       <c r="E47">
@@ -28499,7 +29566,7 @@
         <v>568.21885913853316</v>
       </c>
       <c r="F47">
-        <f>Sheet1!D47</f>
+        <f>Casos!D47</f>
         <v>92472</v>
       </c>
       <c r="G47">
@@ -28507,7 +29574,7 @@
         <v>1528.968253968254</v>
       </c>
       <c r="H47">
-        <f>Sheet1!E47</f>
+        <f>Casos!E47</f>
         <v>52547</v>
       </c>
       <c r="I47">
@@ -28515,7 +29582,7 @@
         <v>634.70225872689934</v>
       </c>
       <c r="J47">
-        <f>Sheet1!F47</f>
+        <f>Casos!F47</f>
         <v>37575</v>
       </c>
       <c r="K47">
@@ -28523,7 +29590,7 @@
         <v>560.90461262875056</v>
       </c>
       <c r="L47">
-        <f>Sheet1!G47</f>
+        <f>Casos!G47</f>
         <v>17089</v>
       </c>
       <c r="M47">
@@ -28546,7 +29613,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <f>Sheet1!B48</f>
+        <f>Casos!B48</f>
         <v>78797</v>
       </c>
       <c r="C48">
@@ -28554,7 +29621,7 @@
         <v>1688.7483926275183</v>
       </c>
       <c r="D48">
-        <f>Sheet1!C48</f>
+        <f>Casos!C48</f>
         <v>10866</v>
       </c>
       <c r="E48">
@@ -28562,7 +29629,7 @@
         <v>632.47962747380677</v>
       </c>
       <c r="F48">
-        <f>Sheet1!D48</f>
+        <f>Casos!D48</f>
         <v>97689</v>
       </c>
       <c r="G48">
@@ -28570,7 +29637,7 @@
         <v>1615.2281746031747</v>
       </c>
       <c r="H48">
-        <f>Sheet1!E48</f>
+        <f>Casos!E48</f>
         <v>57298</v>
       </c>
       <c r="I48">
@@ -28578,7 +29645,7 @@
         <v>692.08841647541965</v>
       </c>
       <c r="J48">
-        <f>Sheet1!F48</f>
+        <f>Casos!F48</f>
         <v>40174</v>
       </c>
       <c r="K48">
@@ -28586,7 +29653,7 @@
         <v>599.70144797731007</v>
       </c>
       <c r="L48">
-        <f>Sheet1!G48</f>
+        <f>Casos!G48</f>
         <v>19522</v>
       </c>
       <c r="M48">
@@ -28594,7 +29661,7 @@
         <v>293.82901866345577</v>
       </c>
       <c r="N48">
-        <f>Sheet1!H49</f>
+        <f>Casos!H49</f>
         <v>143025</v>
       </c>
       <c r="O48">
@@ -28610,7 +29677,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <f>Sheet1!B49</f>
+        <f>Casos!B49</f>
         <v>85195</v>
       </c>
       <c r="C49">
@@ -28618,7 +29685,7 @@
         <v>1825.867981140163</v>
       </c>
       <c r="D49">
-        <f>Sheet1!C49</f>
+        <f>Casos!C49</f>
         <v>11750</v>
       </c>
       <c r="E49">
@@ -28626,7 +29693,7 @@
         <v>683.93480791618163</v>
       </c>
       <c r="F49">
-        <f>Sheet1!D49</f>
+        <f>Casos!D49</f>
         <v>101739</v>
       </c>
       <c r="G49">
@@ -28634,7 +29701,7 @@
         <v>1682.1924603174605</v>
       </c>
       <c r="H49">
-        <f>Sheet1!E49</f>
+        <f>Casos!E49</f>
         <v>61913</v>
       </c>
       <c r="I49">
@@ -28642,7 +29709,7 @@
         <v>747.83186375166076</v>
       </c>
       <c r="J49">
-        <f>Sheet1!F49</f>
+        <f>Casos!F49</f>
         <v>44550</v>
       </c>
       <c r="K49">
@@ -28650,7 +29717,7 @@
         <v>665.02463054187194</v>
       </c>
       <c r="L49">
-        <f>Sheet1!G49</f>
+        <f>Casos!G49</f>
         <v>22141</v>
       </c>
       <c r="M49">
@@ -28658,7 +29725,7 @@
         <v>333.2480433473811</v>
       </c>
       <c r="N49">
-        <f>Sheet1!H50</f>
+        <f>Casos!H50</f>
         <v>163539</v>
       </c>
       <c r="O49">
@@ -28674,7 +29741,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <f>Sheet1!B50</f>
+        <f>Casos!B50</f>
         <v>94417</v>
       </c>
       <c r="C50">
@@ -28682,7 +29749,7 @@
         <v>2023.5105015002146</v>
       </c>
       <c r="D50">
-        <f>Sheet1!C50</f>
+        <f>Casos!C50</f>
         <v>12595</v>
       </c>
       <c r="E50">
@@ -28690,7 +29757,7 @@
         <v>733.11990686845172</v>
       </c>
       <c r="F50">
-        <f>Sheet1!D50</f>
+        <f>Casos!D50</f>
         <v>105792</v>
       </c>
       <c r="G50">
@@ -28698,7 +29765,7 @@
         <v>1749.2063492063494</v>
       </c>
       <c r="H50">
-        <f>Sheet1!E50</f>
+        <f>Casos!E50</f>
         <v>67366</v>
       </c>
       <c r="I50">
@@ -28706,7 +29773,7 @@
         <v>813.6973064379755</v>
       </c>
       <c r="J50">
-        <f>Sheet1!F50</f>
+        <f>Casos!F50</f>
         <v>52128</v>
       </c>
       <c r="K50">
@@ -28714,7 +29781,7 @@
         <v>778.14599193909544</v>
       </c>
       <c r="L50">
-        <f>Sheet1!G50</f>
+        <f>Casos!G50</f>
         <v>25150</v>
       </c>
       <c r="M50">
@@ -28722,7 +29789,7 @@
         <v>378.53702588801929</v>
       </c>
       <c r="N50">
-        <f>Sheet1!H51</f>
+        <f>Casos!H51</f>
         <v>186101</v>
       </c>
       <c r="O50">
@@ -28738,7 +29805,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <f>Sheet1!B51</f>
+        <f>Casos!B51</f>
         <v>102136</v>
       </c>
       <c r="C51">
@@ -28746,7 +29813,7 @@
         <v>2188.9412773253325</v>
       </c>
       <c r="D51">
-        <f>Sheet1!C51</f>
+        <f>Casos!C51</f>
         <v>13614</v>
       </c>
       <c r="E51">
@@ -28754,7 +29821,7 @@
         <v>792.43306169965081</v>
       </c>
       <c r="F51">
-        <f>Sheet1!D51</f>
+        <f>Casos!D51</f>
         <v>110574</v>
       </c>
       <c r="G51">
@@ -28762,7 +29829,7 @@
         <v>1828.2738095238096</v>
       </c>
       <c r="H51">
-        <f>Sheet1!E51</f>
+        <f>Casos!E51</f>
         <v>73522</v>
       </c>
       <c r="I51">
@@ -28770,7 +29837,7 @@
         <v>888.05411281555735</v>
       </c>
       <c r="J51">
-        <f>Sheet1!F51</f>
+        <f>Casos!F51</f>
         <v>56989</v>
       </c>
       <c r="K51">
@@ -28778,7 +29845,7 @@
         <v>850.70906105388872</v>
       </c>
       <c r="L51">
-        <f>Sheet1!G51</f>
+        <f>Casos!G51</f>
         <v>29474</v>
       </c>
       <c r="M51">
@@ -28786,7 +29853,7 @@
         <v>443.61830222757379</v>
       </c>
       <c r="N51" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="O51" t="e">
@@ -28802,7 +29869,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <f>Sheet1!B52</f>
+        <f>Casos!B52</f>
         <v>110238</v>
       </c>
       <c r="C52">
@@ -28810,7 +29877,7 @@
         <v>2362.5803686240893</v>
       </c>
       <c r="D52">
-        <f>Sheet1!C52</f>
+        <f>Casos!C52</f>
         <v>13614</v>
       </c>
       <c r="E52">
@@ -28818,7 +29885,7 @@
         <v>792.43306169965081</v>
       </c>
       <c r="F52">
-        <f>Sheet1!D52</f>
+        <f>Casos!D52</f>
         <v>115242</v>
       </c>
       <c r="G52">
@@ -28826,7 +29893,7 @@
         <v>1905.4563492063494</v>
       </c>
       <c r="H52">
-        <f>Sheet1!E52</f>
+        <f>Casos!E52</f>
         <v>73522</v>
       </c>
       <c r="I52">
@@ -28834,7 +29901,7 @@
         <v>888.05411281555735</v>
       </c>
       <c r="J52">
-        <f>Sheet1!F52</f>
+        <f>Casos!F52</f>
         <v>59105</v>
       </c>
       <c r="K52">
@@ -28842,7 +29909,7 @@
         <v>882.29586505448583</v>
       </c>
       <c r="L52">
-        <f>Sheet1!G52</f>
+        <f>Casos!G52</f>
         <v>33718</v>
       </c>
       <c r="M52">
@@ -28850,7 +29917,7 @@
         <v>507.49548464780253</v>
       </c>
       <c r="N52">
-        <f>Sheet1!H52</f>
+        <f>Casos!H52</f>
         <v>213144</v>
       </c>
       <c r="O52">
@@ -28865,7 +29932,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <f>Sheet1!B53</f>
+        <f>Casos!B53</f>
         <v>117710</v>
       </c>
       <c r="C53">
@@ -28873,27 +29940,27 @@
         <v>2522.717531075868</v>
       </c>
       <c r="D53">
-        <f>Sheet1!C53</f>
+        <f>Casos!C53</f>
         <v>15723</v>
       </c>
       <c r="F53">
-        <f>Sheet1!D53</f>
+        <f>Casos!D53</f>
         <v>119827</v>
       </c>
       <c r="H53" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="J53">
-        <f>Sheet1!E53</f>
+        <f>Casos!E53</f>
         <v>79696</v>
       </c>
       <c r="L53">
-        <f>Sheet1!G53</f>
+        <f>Casos!G53</f>
         <v>38168</v>
       </c>
       <c r="N53">
-        <f>Sheet1!H53</f>
+        <f>Casos!H53</f>
         <v>239279</v>
       </c>
     </row>
@@ -28902,31 +29969,31 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <f>Sheet1!B54</f>
+        <f>Casos!B54</f>
         <v>124736</v>
       </c>
       <c r="D54">
-        <f>Sheet1!C54</f>
+        <f>Casos!C54</f>
         <v>16627</v>
       </c>
       <c r="F54" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="H54" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="J54" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="L54" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="N54">
-        <f>Sheet1!H54</f>
+        <f>Casos!H54</f>
         <v>277205</v>
       </c>
     </row>
@@ -28935,31 +30002,31 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <f>Sheet1!B55</f>
+        <f>Casos!B55</f>
         <v>130759</v>
       </c>
       <c r="D55">
-        <f>Sheet1!C55</f>
+        <f>Casos!C55</f>
         <v>17851</v>
       </c>
       <c r="F55">
-        <f>Sheet1!D54</f>
+        <f>Casos!D54</f>
         <v>124632</v>
       </c>
       <c r="H55">
-        <f>Sheet1!E54</f>
+        <f>Casos!E54</f>
         <v>85778</v>
       </c>
       <c r="J55">
-        <f>Sheet1!F54</f>
+        <f>Casos!F54</f>
         <v>68605</v>
       </c>
       <c r="L55">
-        <f>Sheet1!G54</f>
+        <f>Casos!G54</f>
         <v>41903</v>
       </c>
       <c r="N55">
-        <f>Sheet1!H55</f>
+        <f>Casos!H55</f>
         <v>304826</v>
       </c>
     </row>
@@ -28968,31 +30035,31 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <f>Sheet1!B56</f>
+        <f>Casos!B56</f>
         <v>135032</v>
       </c>
       <c r="D56">
-        <f>Sheet1!C56</f>
+        <f>Casos!C56</f>
         <v>17851</v>
       </c>
       <c r="F56">
-        <f>Sheet1!D56</f>
+        <f>Casos!D56</f>
         <v>128948</v>
       </c>
       <c r="H56">
-        <f>Sheet1!F56</f>
+        <f>Casos!F56</f>
         <v>70478</v>
       </c>
       <c r="J56" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="L56">
-        <f>Sheet1!G56</f>
+        <f>Casos!G56</f>
         <v>48451</v>
       </c>
       <c r="N56">
-        <f>Sheet1!H56</f>
+        <f>Casos!H56</f>
         <v>304826</v>
       </c>
     </row>
@@ -29001,31 +30068,31 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <f>Sheet1!B57</f>
+        <f>Casos!B57</f>
         <v>140510</v>
       </c>
       <c r="D57">
-        <f>Sheet1!C57</f>
+        <f>Casos!C57</f>
         <v>18803</v>
       </c>
       <c r="F57">
-        <f>Sheet1!D57</f>
+        <f>Casos!D57</f>
         <v>132547</v>
       </c>
       <c r="H57">
-        <f>Sheet1!E57</f>
+        <f>Casos!E57</f>
         <v>95391</v>
       </c>
       <c r="J57">
-        <f>Sheet1!F57</f>
+        <f>Casos!F57</f>
         <v>74390</v>
       </c>
       <c r="L57">
-        <f>Sheet1!G57</f>
+        <f>Casos!G57</f>
         <v>51608</v>
       </c>
       <c r="N57">
-        <f>Sheet1!H57</f>
+        <f>Casos!H57</f>
         <v>330891</v>
       </c>
     </row>
@@ -29034,31 +30101,31 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <f>Sheet1!B58</f>
+        <f>Casos!B58</f>
         <v>146690</v>
       </c>
       <c r="D58">
-        <f>Sheet1!C58</f>
+        <f>Casos!C58</f>
         <v>19580</v>
       </c>
       <c r="F58">
-        <f>Sheet1!D58</f>
+        <f>Casos!D58</f>
         <v>135586</v>
       </c>
       <c r="H58">
-        <f>Sheet1!E58</f>
+        <f>Casos!E58</f>
         <v>99225</v>
       </c>
       <c r="J58">
-        <f>Sheet1!F58</f>
+        <f>Casos!F58</f>
         <v>78167</v>
       </c>
       <c r="L58">
-        <f>Sheet1!G58</f>
+        <f>Casos!G58</f>
         <v>55242</v>
       </c>
       <c r="N58">
-        <f>Sheet1!H58</f>
+        <f>Casos!H58</f>
         <v>374329</v>
       </c>
     </row>
@@ -29067,31 +30134,31 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <f>Sheet1!B59</f>
+        <f>Casos!B59</f>
         <v>152446</v>
       </c>
       <c r="D59" t="e">
-        <f>Sheet1!#REF!</f>
+        <f>Casos!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="F59">
-        <f>Sheet1!D59</f>
+        <f>Casos!D59</f>
         <v>139422</v>
       </c>
       <c r="H59">
-        <f>Sheet1!E59</f>
+        <f>Casos!E59</f>
         <v>103228</v>
       </c>
       <c r="J59">
-        <f>Sheet1!F59</f>
+        <f>Casos!F59</f>
         <v>82048</v>
       </c>
       <c r="L59">
-        <f>Sheet1!G59</f>
+        <f>Casos!G59</f>
         <v>60733</v>
       </c>
       <c r="N59">
-        <f>Sheet1!C59</f>
+        <f>Casos!C59</f>
         <v>20549</v>
       </c>
     </row>
@@ -29100,31 +30167,31 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <f>Sheet1!B60</f>
+        <f>Casos!B60</f>
         <v>157022</v>
       </c>
       <c r="D60">
-        <f>Sheet1!C60</f>
+        <f>Casos!C60</f>
         <v>21762</v>
       </c>
       <c r="F60">
-        <f>Sheet1!D60</f>
+        <f>Casos!D60</f>
         <v>143626</v>
       </c>
       <c r="H60">
-        <f>Sheet1!E60</f>
+        <f>Casos!E60</f>
         <v>108202</v>
       </c>
       <c r="J60">
-        <f>Sheet1!F60</f>
+        <f>Casos!F60</f>
         <v>86334</v>
       </c>
       <c r="L60">
-        <f>Sheet1!G60</f>
+        <f>Casos!G60</f>
         <v>65077</v>
       </c>
       <c r="N60">
-        <f>Sheet1!H60</f>
+        <f>Casos!H60</f>
         <v>427460</v>
       </c>
     </row>
@@ -29133,31 +30200,31 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <f>Sheet1!B61</f>
+        <f>Casos!B61</f>
         <v>0</v>
       </c>
       <c r="D61">
-        <f>Sheet1!C61</f>
+        <f>Casos!C61</f>
         <v>0</v>
       </c>
       <c r="F61">
-        <f>Sheet1!D61</f>
+        <f>Casos!D61</f>
         <v>0</v>
       </c>
       <c r="H61">
-        <f>Sheet1!E61</f>
+        <f>Casos!E61</f>
         <v>0</v>
       </c>
       <c r="J61">
-        <f>Sheet1!F61</f>
+        <f>Casos!F61</f>
         <v>0</v>
       </c>
       <c r="L61">
-        <f>Sheet1!G61</f>
+        <f>Casos!G61</f>
         <v>0</v>
       </c>
       <c r="N61">
-        <f>Sheet1!H61</f>
+        <f>Casos!H61</f>
         <v>0</v>
       </c>
     </row>
@@ -29166,31 +30233,31 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <f>Sheet1!B62</f>
+        <f>Casos!B62</f>
         <v>0</v>
       </c>
       <c r="D62">
-        <f>Sheet1!C62</f>
+        <f>Casos!C62</f>
         <v>0</v>
       </c>
       <c r="F62">
-        <f>Sheet1!D62</f>
+        <f>Casos!D62</f>
         <v>0</v>
       </c>
       <c r="H62">
-        <f>Sheet1!E62</f>
+        <f>Casos!E62</f>
         <v>0</v>
       </c>
       <c r="J62">
-        <f>Sheet1!F62</f>
+        <f>Casos!F62</f>
         <v>0</v>
       </c>
       <c r="L62">
-        <f>Sheet1!G62</f>
+        <f>Casos!G62</f>
         <v>0</v>
       </c>
       <c r="N62">
-        <f>Sheet1!H62</f>
+        <f>Casos!H62</f>
         <v>0</v>
       </c>
     </row>
@@ -29199,31 +30266,31 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <f>Sheet1!B63</f>
+        <f>Casos!B63</f>
         <v>0</v>
       </c>
       <c r="D63">
-        <f>Sheet1!C63</f>
+        <f>Casos!C63</f>
         <v>0</v>
       </c>
       <c r="F63">
-        <f>Sheet1!D63</f>
+        <f>Casos!D63</f>
         <v>0</v>
       </c>
       <c r="H63">
-        <f>Sheet1!E63</f>
+        <f>Casos!E63</f>
         <v>0</v>
       </c>
       <c r="J63">
-        <f>Sheet1!F63</f>
+        <f>Casos!F63</f>
         <v>0</v>
       </c>
       <c r="L63">
-        <f>Sheet1!G63</f>
+        <f>Casos!G63</f>
         <v>0</v>
       </c>
       <c r="N63">
-        <f>Sheet1!H63</f>
+        <f>Casos!H63</f>
         <v>0</v>
       </c>
     </row>
@@ -29232,31 +30299,31 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <f>Sheet1!B64</f>
+        <f>Casos!B64</f>
         <v>0</v>
       </c>
       <c r="D64">
-        <f>Sheet1!C64</f>
+        <f>Casos!C64</f>
         <v>0</v>
       </c>
       <c r="F64">
-        <f>Sheet1!D64</f>
+        <f>Casos!D64</f>
         <v>0</v>
       </c>
       <c r="H64">
-        <f>Sheet1!E64</f>
+        <f>Casos!E64</f>
         <v>0</v>
       </c>
       <c r="J64">
-        <f>Sheet1!F64</f>
+        <f>Casos!F64</f>
         <v>0</v>
       </c>
       <c r="L64">
-        <f>Sheet1!G64</f>
+        <f>Casos!G64</f>
         <v>0</v>
       </c>
       <c r="N64">
-        <f>Sheet1!H64</f>
+        <f>Casos!H64</f>
         <v>0</v>
       </c>
     </row>
@@ -29265,31 +30332,31 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <f>Sheet1!B65</f>
+        <f>Casos!B65</f>
         <v>0</v>
       </c>
       <c r="D65">
-        <f>Sheet1!C65</f>
+        <f>Casos!C65</f>
         <v>0</v>
       </c>
       <c r="F65">
-        <f>Sheet1!D65</f>
+        <f>Casos!D65</f>
         <v>0</v>
       </c>
       <c r="H65">
-        <f>Sheet1!E65</f>
+        <f>Casos!E65</f>
         <v>0</v>
       </c>
       <c r="J65">
-        <f>Sheet1!F65</f>
+        <f>Casos!F65</f>
         <v>0</v>
       </c>
       <c r="L65">
-        <f>Sheet1!G65</f>
+        <f>Casos!G65</f>
         <v>0</v>
       </c>
       <c r="N65">
-        <f>Sheet1!H65</f>
+        <f>Casos!H65</f>
         <v>0</v>
       </c>
     </row>
@@ -29298,31 +30365,31 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <f>Sheet1!B66</f>
+        <f>Casos!B66</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f>Sheet1!C66</f>
+        <f>Casos!C66</f>
         <v>0</v>
       </c>
       <c r="F66">
-        <f>Sheet1!D66</f>
+        <f>Casos!D66</f>
         <v>0</v>
       </c>
       <c r="H66">
-        <f>Sheet1!E66</f>
+        <f>Casos!E66</f>
         <v>0</v>
       </c>
       <c r="J66">
-        <f>Sheet1!F66</f>
+        <f>Casos!F66</f>
         <v>0</v>
       </c>
       <c r="L66">
-        <f>Sheet1!G66</f>
+        <f>Casos!G66</f>
         <v>0</v>
       </c>
       <c r="N66">
-        <f>Sheet1!H66</f>
+        <f>Casos!H66</f>
         <v>0</v>
       </c>
     </row>
@@ -29331,31 +30398,31 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <f>Sheet1!B67</f>
+        <f>Casos!B67</f>
         <v>0</v>
       </c>
       <c r="D67">
-        <f>Sheet1!C67</f>
+        <f>Casos!C67</f>
         <v>0</v>
       </c>
       <c r="F67">
-        <f>Sheet1!D67</f>
+        <f>Casos!D67</f>
         <v>0</v>
       </c>
       <c r="H67">
-        <f>Sheet1!E67</f>
+        <f>Casos!E67</f>
         <v>0</v>
       </c>
       <c r="J67">
-        <f>Sheet1!F67</f>
+        <f>Casos!F67</f>
         <v>0</v>
       </c>
       <c r="L67">
-        <f>Sheet1!G67</f>
+        <f>Casos!G67</f>
         <v>0</v>
       </c>
       <c r="N67">
-        <f>Sheet1!H67</f>
+        <f>Casos!H67</f>
         <v>0</v>
       </c>
     </row>
@@ -29364,31 +30431,31 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <f>Sheet1!B68</f>
+        <f>Casos!B68</f>
         <v>0</v>
       </c>
       <c r="D68">
-        <f>Sheet1!C68</f>
+        <f>Casos!C68</f>
         <v>0</v>
       </c>
       <c r="F68">
-        <f>Sheet1!D68</f>
+        <f>Casos!D68</f>
         <v>0</v>
       </c>
       <c r="H68">
-        <f>Sheet1!E68</f>
+        <f>Casos!E68</f>
         <v>0</v>
       </c>
       <c r="J68">
-        <f>Sheet1!F68</f>
+        <f>Casos!F68</f>
         <v>0</v>
       </c>
       <c r="L68">
-        <f>Sheet1!G68</f>
+        <f>Casos!G68</f>
         <v>0</v>
       </c>
       <c r="N68">
-        <f>Sheet1!H68</f>
+        <f>Casos!H68</f>
         <v>0</v>
       </c>
     </row>
@@ -29397,31 +30464,31 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <f>Sheet1!B69</f>
+        <f>Casos!B69</f>
         <v>0</v>
       </c>
       <c r="D69">
-        <f>Sheet1!C69</f>
+        <f>Casos!C69</f>
         <v>0</v>
       </c>
       <c r="F69">
-        <f>Sheet1!D69</f>
+        <f>Casos!D69</f>
         <v>0</v>
       </c>
       <c r="H69">
-        <f>Sheet1!E69</f>
+        <f>Casos!E69</f>
         <v>0</v>
       </c>
       <c r="J69">
-        <f>Sheet1!F69</f>
+        <f>Casos!F69</f>
         <v>0</v>
       </c>
       <c r="L69">
-        <f>Sheet1!G69</f>
+        <f>Casos!G69</f>
         <v>0</v>
       </c>
       <c r="N69">
-        <f>Sheet1!H69</f>
+        <f>Casos!H69</f>
         <v>0</v>
       </c>
     </row>
@@ -29430,31 +30497,31 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <f>Sheet1!B70</f>
+        <f>Casos!B70</f>
         <v>0</v>
       </c>
       <c r="D70">
-        <f>Sheet1!C70</f>
+        <f>Casos!C70</f>
         <v>0</v>
       </c>
       <c r="F70">
-        <f>Sheet1!D70</f>
+        <f>Casos!D70</f>
         <v>0</v>
       </c>
       <c r="H70">
-        <f>Sheet1!E70</f>
+        <f>Casos!E70</f>
         <v>0</v>
       </c>
       <c r="J70">
-        <f>Sheet1!F70</f>
+        <f>Casos!F70</f>
         <v>0</v>
       </c>
       <c r="L70">
-        <f>Sheet1!G70</f>
+        <f>Casos!G70</f>
         <v>0</v>
       </c>
       <c r="N70">
-        <f>Sheet1!H70</f>
+        <f>Casos!H70</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update fixing wrong data on Italy 14/04
</commit_message>
<xml_diff>
--- a/Sources/Paises.xlsx
+++ b/Sources/Paises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\PowerBI_Covid\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB495C4-9310-4E39-8B8D-7943EFC65054}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E860CCA-D5DB-496F-8C67-EA7CC77FA811}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
   <si>
     <t>Italia</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>Fallecidos</t>
-  </si>
-  <si>
-    <t>159.516 I</t>
   </si>
 </sst>
 </file>
@@ -15819,7 +15816,7 @@
   <dimension ref="A1:AL70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18913,8 +18910,8 @@
       <c r="C64">
         <v>26551</v>
       </c>
-      <c r="D64" t="s">
-        <v>48</v>
+      <c r="D64">
+        <v>159516</v>
       </c>
       <c r="E64">
         <v>123016</v>
@@ -23987,9 +23984,9 @@
         <f>Casos!C64</f>
         <v>26551</v>
       </c>
-      <c r="F64" t="str">
+      <c r="F64">
         <f>Casos!D64</f>
-        <v>159.516 I</v>
+        <v>159516</v>
       </c>
       <c r="H64">
         <f>Casos!E64</f>
@@ -27295,9 +27292,9 @@
         <f>Casos!C64</f>
         <v>26551</v>
       </c>
-      <c r="F64" t="str">
+      <c r="F64">
         <f>Casos!D64</f>
-        <v>159.516 I</v>
+        <v>159516</v>
       </c>
       <c r="H64">
         <f>Casos!E64</f>
@@ -30579,9 +30576,9 @@
         <f>Casos!C64</f>
         <v>26551</v>
       </c>
-      <c r="F64" t="str">
+      <c r="F64">
         <f>Casos!D64</f>
-        <v>159.516 I</v>
+        <v>159516</v>
       </c>
       <c r="H64">
         <f>Casos!E64</f>

</xml_diff>